<commit_message>
fix update database monthly
</commit_message>
<xml_diff>
--- a/database/industries/darou/deabid/product/monthly.xlsx
+++ b/database/industries/darou/deabid/product/monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="e:\Trade\database\industries\darou\deabid\product\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F97D01-DFEB-4F08-AFF4-3EC90A98FC42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2972B9-7BB0-4CE2-B7CB-F106C82663C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2640" yWindow="1704" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="91">
   <si>
     <t>Pouya Finance</t>
   </si>
   <si>
-    <t>Copyright @2015 - 2022</t>
+    <t>Copyright @2015 - 2023</t>
   </si>
   <si>
     <t>دعبید-لابراتوارداروسازی‌  دکترعبیدی‌</t>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>مقدار تولید</t>
-  </si>
-  <si>
-    <t>ماه 10 منتهی به 1397/07</t>
   </si>
   <si>
     <t>ماه 11 منتهی به 1397/08</t>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>ماه 11 منتهی به 1401/08</t>
+  </si>
+  <si>
+    <t>ماه 12 منتهی به 1401/09</t>
   </si>
   <si>
     <t>سایر</t>
@@ -1564,8 +1564,8 @@
       <c r="AP11" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AQ11" s="11" t="s">
-        <v>57</v>
+      <c r="AQ11" s="11">
+        <v>0</v>
       </c>
       <c r="AR11" s="11">
         <v>0</v>
@@ -1577,22 +1577,22 @@
         <v>0</v>
       </c>
       <c r="AU11" s="11">
-        <v>0</v>
+        <v>170889</v>
       </c>
       <c r="AV11" s="11">
-        <v>170889</v>
+        <v>47524</v>
       </c>
       <c r="AW11" s="11">
-        <v>47524</v>
+        <v>6273</v>
       </c>
       <c r="AX11" s="11">
-        <v>6273</v>
+        <v>432</v>
       </c>
       <c r="AY11" s="11">
-        <v>432</v>
+        <v>3469</v>
       </c>
       <c r="AZ11" s="11">
-        <v>3469</v>
+        <v>0</v>
       </c>
       <c r="BA11" s="11">
         <v>0</v>
@@ -1633,62 +1633,62 @@
       <c r="L12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="13" t="s">
-        <v>57</v>
+      <c r="M12" s="13">
+        <v>23700</v>
       </c>
       <c r="N12" s="13">
-        <v>23700</v>
+        <v>18195</v>
       </c>
       <c r="O12" s="13">
-        <v>18195</v>
+        <v>95472</v>
       </c>
       <c r="P12" s="13">
-        <v>95472</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="13">
         <v>0</v>
       </c>
       <c r="R12" s="13">
-        <v>0</v>
-      </c>
-      <c r="S12" s="13">
         <v>64485</v>
       </c>
+      <c r="S12" s="13" t="s">
+        <v>57</v>
+      </c>
       <c r="T12" s="13" t="s">
         <v>57</v>
       </c>
       <c r="U12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="V12" s="13" t="s">
-        <v>57</v>
+      <c r="V12" s="13">
+        <v>9600</v>
       </c>
       <c r="W12" s="13">
-        <v>9600</v>
+        <v>122849</v>
       </c>
       <c r="X12" s="13">
-        <v>122849</v>
+        <v>264</v>
       </c>
       <c r="Y12" s="13">
-        <v>264</v>
+        <v>47661</v>
       </c>
       <c r="Z12" s="13">
-        <v>47661</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="13">
         <v>0</v>
       </c>
       <c r="AB12" s="13">
-        <v>0</v>
+        <v>62929</v>
       </c>
       <c r="AC12" s="13">
-        <v>62929</v>
+        <v>69520</v>
       </c>
       <c r="AD12" s="13">
-        <v>69520</v>
-      </c>
-      <c r="AE12" s="13">
         <v>107334</v>
+      </c>
+      <c r="AE12" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AF12" s="13" t="s">
         <v>57</v>
@@ -1769,34 +1769,34 @@
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="11">
-        <v>26431</v>
+        <v>0</v>
       </c>
       <c r="F13" s="11">
         <v>0</v>
       </c>
       <c r="G13" s="11">
-        <v>0</v>
+        <v>15568</v>
       </c>
       <c r="H13" s="11">
-        <v>15568</v>
+        <v>0</v>
       </c>
       <c r="I13" s="11">
         <v>0</v>
       </c>
       <c r="J13" s="11">
-        <v>0</v>
+        <v>9360</v>
       </c>
       <c r="K13" s="11">
-        <v>9360</v>
+        <v>37764</v>
       </c>
       <c r="L13" s="11">
-        <v>37764</v>
+        <v>0</v>
       </c>
       <c r="M13" s="11">
-        <v>0</v>
+        <v>31375</v>
       </c>
       <c r="N13" s="11">
-        <v>31375</v>
+        <v>0</v>
       </c>
       <c r="O13" s="11">
         <v>0</v>
@@ -1817,11 +1817,11 @@
         <v>0</v>
       </c>
       <c r="U13" s="11">
-        <v>0</v>
-      </c>
-      <c r="V13" s="11">
         <v>95541</v>
       </c>
+      <c r="V13" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="W13" s="11" t="s">
         <v>57</v>
       </c>
@@ -1846,35 +1846,35 @@
       <c r="AD13" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AE13" s="11" t="s">
-        <v>57</v>
+      <c r="AE13" s="11">
+        <v>181992</v>
       </c>
       <c r="AF13" s="11">
-        <v>181992</v>
+        <v>147483</v>
       </c>
       <c r="AG13" s="11">
-        <v>147483</v>
+        <v>56346</v>
       </c>
       <c r="AH13" s="11">
-        <v>56346</v>
+        <v>27294</v>
       </c>
       <c r="AI13" s="11">
-        <v>27294</v>
+        <v>110256</v>
       </c>
       <c r="AJ13" s="11">
-        <v>110256</v>
+        <v>145656</v>
       </c>
       <c r="AK13" s="11">
-        <v>145656</v>
+        <v>133179</v>
       </c>
       <c r="AL13" s="11">
-        <v>133179</v>
+        <v>82248</v>
       </c>
       <c r="AM13" s="11">
-        <v>82248</v>
+        <v>118200</v>
       </c>
       <c r="AN13" s="11">
-        <v>118200</v>
+        <v>0</v>
       </c>
       <c r="AO13" s="11">
         <v>0</v>
@@ -1882,8 +1882,8 @@
       <c r="AP13" s="11">
         <v>0</v>
       </c>
-      <c r="AQ13" s="11">
-        <v>0</v>
+      <c r="AQ13" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="AR13" s="11" t="s">
         <v>57</v>
@@ -1928,121 +1928,121 @@
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13">
-        <v>1009673</v>
+        <v>1081099</v>
       </c>
       <c r="F14" s="13">
-        <v>1081099</v>
+        <v>637316</v>
       </c>
       <c r="G14" s="13">
-        <v>637316</v>
+        <v>1141442</v>
       </c>
       <c r="H14" s="13">
-        <v>1141442</v>
+        <v>1337266</v>
       </c>
       <c r="I14" s="13">
-        <v>1337266</v>
+        <v>1007290</v>
       </c>
       <c r="J14" s="13">
-        <v>1007290</v>
+        <v>589339</v>
       </c>
       <c r="K14" s="13">
-        <v>589339</v>
+        <v>1145715</v>
       </c>
       <c r="L14" s="13">
-        <v>1145715</v>
+        <v>431841</v>
       </c>
       <c r="M14" s="13">
-        <v>431841</v>
+        <v>811001</v>
       </c>
       <c r="N14" s="13">
-        <v>811001</v>
+        <v>1284602</v>
       </c>
       <c r="O14" s="13">
-        <v>1284602</v>
+        <v>1499096</v>
       </c>
       <c r="P14" s="13">
-        <v>1499096</v>
+        <v>1584000</v>
       </c>
       <c r="Q14" s="13">
-        <v>1584000</v>
+        <v>1174611</v>
       </c>
       <c r="R14" s="13">
-        <v>1174611</v>
+        <v>1081207</v>
       </c>
       <c r="S14" s="13">
-        <v>1081207</v>
+        <v>921990</v>
       </c>
       <c r="T14" s="13">
-        <v>921990</v>
+        <v>1373295</v>
       </c>
       <c r="U14" s="13">
-        <v>1373295</v>
+        <v>1113756</v>
       </c>
       <c r="V14" s="13">
-        <v>1113756</v>
+        <v>657907</v>
       </c>
       <c r="W14" s="13">
-        <v>657907</v>
+        <v>946203</v>
       </c>
       <c r="X14" s="13">
-        <v>946203</v>
+        <v>1009668</v>
       </c>
       <c r="Y14" s="13">
-        <v>1009668</v>
+        <v>1174421</v>
       </c>
       <c r="Z14" s="13">
-        <v>1174421</v>
+        <v>413674</v>
       </c>
       <c r="AA14" s="13">
-        <v>413674</v>
+        <v>643438</v>
       </c>
       <c r="AB14" s="13">
-        <v>643438</v>
+        <v>711664</v>
       </c>
       <c r="AC14" s="13">
-        <v>711664</v>
+        <v>657418</v>
       </c>
       <c r="AD14" s="13">
-        <v>657418</v>
+        <v>454086</v>
       </c>
       <c r="AE14" s="13">
-        <v>454086</v>
+        <v>0</v>
       </c>
       <c r="AF14" s="13">
         <v>0</v>
       </c>
       <c r="AG14" s="13">
-        <v>0</v>
+        <v>648758</v>
       </c>
       <c r="AH14" s="13">
-        <v>648758</v>
+        <v>347225</v>
       </c>
       <c r="AI14" s="13">
-        <v>347225</v>
+        <v>400294</v>
       </c>
       <c r="AJ14" s="13">
-        <v>400294</v>
+        <v>389635</v>
       </c>
       <c r="AK14" s="13">
-        <v>389635</v>
+        <v>163886</v>
       </c>
       <c r="AL14" s="13">
-        <v>163886</v>
+        <v>782691</v>
       </c>
       <c r="AM14" s="13">
-        <v>782691</v>
+        <v>1244376</v>
       </c>
       <c r="AN14" s="13">
-        <v>1244376</v>
+        <v>1346164</v>
       </c>
       <c r="AO14" s="13">
-        <v>1346164</v>
+        <v>1177885</v>
       </c>
       <c r="AP14" s="13">
-        <v>1177885</v>
-      </c>
-      <c r="AQ14" s="13">
         <v>1315827</v>
+      </c>
+      <c r="AQ14" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AR14" s="13" t="s">
         <v>57</v>
@@ -2087,154 +2087,154 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11">
-        <v>229162</v>
+        <v>300424</v>
       </c>
       <c r="F15" s="11">
-        <v>300424</v>
+        <v>397095</v>
       </c>
       <c r="G15" s="11">
-        <v>397095</v>
+        <v>626128</v>
       </c>
       <c r="H15" s="11">
-        <v>626128</v>
+        <v>374448</v>
       </c>
       <c r="I15" s="11">
-        <v>374448</v>
+        <v>581643</v>
       </c>
       <c r="J15" s="11">
-        <v>581643</v>
+        <v>427973</v>
       </c>
       <c r="K15" s="11">
-        <v>427973</v>
+        <v>477029</v>
       </c>
       <c r="L15" s="11">
-        <v>477029</v>
+        <v>525169</v>
       </c>
       <c r="M15" s="11">
-        <v>525169</v>
+        <v>605197</v>
       </c>
       <c r="N15" s="11">
-        <v>605197</v>
+        <v>119197</v>
       </c>
       <c r="O15" s="11">
-        <v>119197</v>
+        <v>573335</v>
       </c>
       <c r="P15" s="11">
-        <v>573335</v>
+        <v>618345</v>
       </c>
       <c r="Q15" s="11">
-        <v>618345</v>
+        <v>548175</v>
       </c>
       <c r="R15" s="11">
-        <v>548175</v>
+        <v>427794</v>
       </c>
       <c r="S15" s="11">
-        <v>427794</v>
+        <v>539973</v>
       </c>
       <c r="T15" s="11">
-        <v>539973</v>
+        <v>350082</v>
       </c>
       <c r="U15" s="11">
-        <v>350082</v>
+        <v>337868</v>
       </c>
       <c r="V15" s="11">
-        <v>337868</v>
+        <v>204506</v>
       </c>
       <c r="W15" s="11">
-        <v>204506</v>
+        <v>318686</v>
       </c>
       <c r="X15" s="11">
-        <v>318686</v>
+        <v>281246</v>
       </c>
       <c r="Y15" s="11">
-        <v>281246</v>
+        <v>727175</v>
       </c>
       <c r="Z15" s="11">
-        <v>727175</v>
+        <v>538233</v>
       </c>
       <c r="AA15" s="11">
-        <v>538233</v>
+        <v>855005</v>
       </c>
       <c r="AB15" s="11">
-        <v>855005</v>
+        <v>632026</v>
       </c>
       <c r="AC15" s="11">
-        <v>632026</v>
+        <v>378438</v>
       </c>
       <c r="AD15" s="11">
-        <v>378438</v>
+        <v>517873</v>
       </c>
       <c r="AE15" s="11">
-        <v>517873</v>
+        <v>560590</v>
       </c>
       <c r="AF15" s="11">
-        <v>560590</v>
+        <v>838639</v>
       </c>
       <c r="AG15" s="11">
-        <v>838639</v>
+        <v>767371</v>
       </c>
       <c r="AH15" s="11">
-        <v>767371</v>
+        <v>632517</v>
       </c>
       <c r="AI15" s="11">
-        <v>632517</v>
+        <v>613162</v>
       </c>
       <c r="AJ15" s="11">
-        <v>613162</v>
+        <v>714062</v>
       </c>
       <c r="AK15" s="11">
-        <v>714062</v>
+        <v>661344</v>
       </c>
       <c r="AL15" s="11">
-        <v>661344</v>
+        <v>770553</v>
       </c>
       <c r="AM15" s="11">
-        <v>770553</v>
+        <v>1135161</v>
       </c>
       <c r="AN15" s="11">
-        <v>1135161</v>
+        <v>819172</v>
       </c>
       <c r="AO15" s="11">
-        <v>819172</v>
+        <v>838951</v>
       </c>
       <c r="AP15" s="11">
-        <v>838951</v>
+        <v>479861</v>
       </c>
       <c r="AQ15" s="11">
-        <v>479861</v>
+        <v>588260</v>
       </c>
       <c r="AR15" s="11">
-        <v>588260</v>
+        <v>721986</v>
       </c>
       <c r="AS15" s="11">
-        <v>721986</v>
+        <v>539519</v>
       </c>
       <c r="AT15" s="11">
-        <v>539519</v>
+        <v>404238</v>
       </c>
       <c r="AU15" s="11">
-        <v>404238</v>
+        <v>741943</v>
       </c>
       <c r="AV15" s="11">
-        <v>741943</v>
+        <v>650106</v>
       </c>
       <c r="AW15" s="11">
-        <v>650106</v>
+        <v>718497</v>
       </c>
       <c r="AX15" s="11">
-        <v>718497</v>
+        <v>566655</v>
       </c>
       <c r="AY15" s="11">
-        <v>566655</v>
+        <v>991067</v>
       </c>
       <c r="AZ15" s="11">
-        <v>991067</v>
+        <v>723241</v>
       </c>
       <c r="BA15" s="11">
-        <v>723241</v>
+        <v>881696</v>
       </c>
       <c r="BB15" s="11">
-        <v>881696</v>
+        <v>579664</v>
       </c>
     </row>
     <row r="16" spans="2:54" x14ac:dyDescent="0.3">
@@ -2246,154 +2246,154 @@
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="13">
-        <v>1831142</v>
+        <v>2277316</v>
       </c>
       <c r="F16" s="13">
-        <v>2277316</v>
+        <v>2201105</v>
       </c>
       <c r="G16" s="13">
-        <v>2201105</v>
+        <v>2166819</v>
       </c>
       <c r="H16" s="13">
-        <v>2166819</v>
+        <v>2847184</v>
       </c>
       <c r="I16" s="13">
-        <v>2847184</v>
+        <v>1314946</v>
       </c>
       <c r="J16" s="13">
-        <v>1314946</v>
+        <v>1291472</v>
       </c>
       <c r="K16" s="13">
-        <v>1291472</v>
+        <v>2152965</v>
       </c>
       <c r="L16" s="13">
-        <v>2152965</v>
+        <v>2246598</v>
       </c>
       <c r="M16" s="13">
-        <v>2246598</v>
+        <v>1685872</v>
       </c>
       <c r="N16" s="13">
-        <v>1685872</v>
+        <v>1106551</v>
       </c>
       <c r="O16" s="13">
-        <v>1106551</v>
+        <v>1413553</v>
       </c>
       <c r="P16" s="13">
-        <v>1413553</v>
+        <v>1998291</v>
       </c>
       <c r="Q16" s="13">
-        <v>1998291</v>
+        <v>1911875</v>
       </c>
       <c r="R16" s="13">
-        <v>1911875</v>
+        <v>2265924</v>
       </c>
       <c r="S16" s="13">
-        <v>2265924</v>
+        <v>2040424</v>
       </c>
       <c r="T16" s="13">
-        <v>2040424</v>
+        <v>2594624</v>
       </c>
       <c r="U16" s="13">
-        <v>2594624</v>
+        <v>1815057</v>
       </c>
       <c r="V16" s="13">
-        <v>1815057</v>
+        <v>1282858</v>
       </c>
       <c r="W16" s="13">
-        <v>1282858</v>
+        <v>2462563</v>
       </c>
       <c r="X16" s="13">
-        <v>2462563</v>
+        <v>2135420</v>
       </c>
       <c r="Y16" s="13">
-        <v>2135420</v>
+        <v>2038745</v>
       </c>
       <c r="Z16" s="13">
-        <v>2038745</v>
+        <v>2166318</v>
       </c>
       <c r="AA16" s="13">
-        <v>2166318</v>
+        <v>1658517</v>
       </c>
       <c r="AB16" s="13">
-        <v>1658517</v>
+        <v>2655399</v>
       </c>
       <c r="AC16" s="13">
-        <v>2655399</v>
+        <v>2484030</v>
       </c>
       <c r="AD16" s="13">
-        <v>2484030</v>
+        <v>2000890</v>
       </c>
       <c r="AE16" s="13">
-        <v>2000890</v>
+        <v>2501078</v>
       </c>
       <c r="AF16" s="13">
-        <v>2501078</v>
+        <v>2206098</v>
       </c>
       <c r="AG16" s="13">
-        <v>2206098</v>
+        <v>2446312</v>
       </c>
       <c r="AH16" s="13">
-        <v>2446312</v>
+        <v>1153464</v>
       </c>
       <c r="AI16" s="13">
-        <v>1153464</v>
+        <v>1890019</v>
       </c>
       <c r="AJ16" s="13">
-        <v>1890019</v>
+        <v>1928260</v>
       </c>
       <c r="AK16" s="13">
-        <v>1928260</v>
+        <v>1713709</v>
       </c>
       <c r="AL16" s="13">
-        <v>1713709</v>
+        <v>1958099</v>
       </c>
       <c r="AM16" s="13">
-        <v>1958099</v>
+        <v>1784095</v>
       </c>
       <c r="AN16" s="13">
-        <v>1784095</v>
+        <v>1713376</v>
       </c>
       <c r="AO16" s="13">
-        <v>1713376</v>
+        <v>1278960</v>
       </c>
       <c r="AP16" s="13">
-        <v>1278960</v>
+        <v>1702921</v>
       </c>
       <c r="AQ16" s="13">
-        <v>1702921</v>
+        <v>2394727</v>
       </c>
       <c r="AR16" s="13">
-        <v>2394727</v>
+        <v>2472522</v>
       </c>
       <c r="AS16" s="13">
-        <v>2472522</v>
+        <v>2648824</v>
       </c>
       <c r="AT16" s="13">
-        <v>2648824</v>
+        <v>2467148</v>
       </c>
       <c r="AU16" s="13">
-        <v>2467148</v>
+        <v>2259761</v>
       </c>
       <c r="AV16" s="13">
-        <v>2259761</v>
+        <v>2413870</v>
       </c>
       <c r="AW16" s="13">
-        <v>2413870</v>
+        <v>3150200</v>
       </c>
       <c r="AX16" s="13">
-        <v>3150200</v>
+        <v>3041277</v>
       </c>
       <c r="AY16" s="13">
-        <v>3041277</v>
+        <v>2868961</v>
       </c>
       <c r="AZ16" s="13">
-        <v>2868961</v>
+        <v>3361887</v>
       </c>
       <c r="BA16" s="13">
-        <v>3361887</v>
+        <v>2860358</v>
       </c>
       <c r="BB16" s="13">
-        <v>2860358</v>
+        <v>3502147</v>
       </c>
     </row>
     <row r="17" spans="2:54" x14ac:dyDescent="0.3">
@@ -2410,8 +2410,8 @@
       <c r="F17" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>57</v>
+      <c r="G17" s="11">
+        <v>0</v>
       </c>
       <c r="H17" s="11">
         <v>0</v>
@@ -2446,8 +2446,8 @@
       <c r="R17" s="11">
         <v>0</v>
       </c>
-      <c r="S17" s="11">
-        <v>0</v>
+      <c r="S17" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="T17" s="11" t="s">
         <v>57</v>
@@ -2677,41 +2677,41 @@
       <c r="AP18" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AQ18" s="13" t="s">
-        <v>57</v>
+      <c r="AQ18" s="13">
+        <v>1585260</v>
       </c>
       <c r="AR18" s="13">
-        <v>1585260</v>
+        <v>1421117</v>
       </c>
       <c r="AS18" s="13">
-        <v>1421117</v>
+        <v>1557544</v>
       </c>
       <c r="AT18" s="13">
-        <v>1557544</v>
+        <v>1305324</v>
       </c>
       <c r="AU18" s="13">
-        <v>1305324</v>
+        <v>1503893</v>
       </c>
       <c r="AV18" s="13">
-        <v>1503893</v>
+        <v>1171549</v>
       </c>
       <c r="AW18" s="13">
-        <v>1171549</v>
+        <v>1388134</v>
       </c>
       <c r="AX18" s="13">
-        <v>1388134</v>
+        <v>1505023</v>
       </c>
       <c r="AY18" s="13">
-        <v>1505023</v>
+        <v>1602370</v>
       </c>
       <c r="AZ18" s="13">
-        <v>1602370</v>
+        <v>1522111</v>
       </c>
       <c r="BA18" s="13">
-        <v>1522111</v>
+        <v>2021194</v>
       </c>
       <c r="BB18" s="13">
-        <v>2021194</v>
+        <v>1892337</v>
       </c>
     </row>
     <row r="19" spans="2:54" x14ac:dyDescent="0.3">
@@ -2855,8 +2855,8 @@
       <c r="AD20" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AE20" s="17" t="s">
-        <v>57</v>
+      <c r="AE20" s="17">
+        <v>0</v>
       </c>
       <c r="AF20" s="17">
         <v>0</v>
@@ -2935,154 +2935,154 @@
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19">
-        <v>3096408</v>
+        <v>3658839</v>
       </c>
       <c r="F21" s="19">
-        <v>3658839</v>
+        <v>3235516</v>
       </c>
       <c r="G21" s="19">
-        <v>3235516</v>
+        <v>3949957</v>
       </c>
       <c r="H21" s="19">
-        <v>3949957</v>
+        <v>4558898</v>
       </c>
       <c r="I21" s="19">
-        <v>4558898</v>
+        <v>2903879</v>
       </c>
       <c r="J21" s="19">
-        <v>2903879</v>
+        <v>2318144</v>
       </c>
       <c r="K21" s="19">
-        <v>2318144</v>
+        <v>3813473</v>
       </c>
       <c r="L21" s="19">
-        <v>3813473</v>
+        <v>3203608</v>
       </c>
       <c r="M21" s="19">
-        <v>3203608</v>
+        <v>3157145</v>
       </c>
       <c r="N21" s="19">
-        <v>3157145</v>
+        <v>2528545</v>
       </c>
       <c r="O21" s="19">
-        <v>2528545</v>
+        <v>3581456</v>
       </c>
       <c r="P21" s="19">
-        <v>3581456</v>
+        <v>4200636</v>
       </c>
       <c r="Q21" s="19">
-        <v>4200636</v>
+        <v>3634661</v>
       </c>
       <c r="R21" s="19">
-        <v>3634661</v>
+        <v>3839410</v>
       </c>
       <c r="S21" s="19">
-        <v>3839410</v>
+        <v>3502387</v>
       </c>
       <c r="T21" s="19">
-        <v>3502387</v>
+        <v>4318001</v>
       </c>
       <c r="U21" s="19">
-        <v>4318001</v>
+        <v>3362222</v>
       </c>
       <c r="V21" s="19">
-        <v>3362222</v>
+        <v>2154871</v>
       </c>
       <c r="W21" s="19">
-        <v>2154871</v>
+        <v>3850301</v>
       </c>
       <c r="X21" s="19">
-        <v>3850301</v>
+        <v>3426598</v>
       </c>
       <c r="Y21" s="19">
-        <v>3426598</v>
+        <v>3988002</v>
       </c>
       <c r="Z21" s="19">
-        <v>3988002</v>
+        <v>3118225</v>
       </c>
       <c r="AA21" s="19">
-        <v>3118225</v>
+        <v>3156960</v>
       </c>
       <c r="AB21" s="19">
-        <v>3156960</v>
+        <v>4062018</v>
       </c>
       <c r="AC21" s="19">
-        <v>4062018</v>
+        <v>3589406</v>
       </c>
       <c r="AD21" s="19">
-        <v>3589406</v>
+        <v>3080183</v>
       </c>
       <c r="AE21" s="19">
-        <v>3080183</v>
+        <v>3243660</v>
       </c>
       <c r="AF21" s="19">
-        <v>3243660</v>
+        <v>3192220</v>
       </c>
       <c r="AG21" s="19">
-        <v>3192220</v>
+        <v>3918787</v>
       </c>
       <c r="AH21" s="19">
-        <v>3918787</v>
+        <v>2160500</v>
       </c>
       <c r="AI21" s="19">
-        <v>2160500</v>
+        <v>3013731</v>
       </c>
       <c r="AJ21" s="19">
-        <v>3013731</v>
+        <v>3177613</v>
       </c>
       <c r="AK21" s="19">
-        <v>3177613</v>
+        <v>2672118</v>
       </c>
       <c r="AL21" s="19">
-        <v>2672118</v>
+        <v>3593591</v>
       </c>
       <c r="AM21" s="19">
-        <v>3593591</v>
+        <v>4281832</v>
       </c>
       <c r="AN21" s="19">
-        <v>4281832</v>
+        <v>3878712</v>
       </c>
       <c r="AO21" s="19">
-        <v>3878712</v>
+        <v>3295796</v>
       </c>
       <c r="AP21" s="19">
-        <v>3295796</v>
+        <v>3498609</v>
       </c>
       <c r="AQ21" s="19">
-        <v>3498609</v>
+        <v>4568247</v>
       </c>
       <c r="AR21" s="19">
-        <v>4568247</v>
+        <v>4615625</v>
       </c>
       <c r="AS21" s="19">
-        <v>4615625</v>
+        <v>4745887</v>
       </c>
       <c r="AT21" s="19">
-        <v>4745887</v>
+        <v>4176710</v>
       </c>
       <c r="AU21" s="19">
-        <v>4176710</v>
+        <v>4676486</v>
       </c>
       <c r="AV21" s="19">
-        <v>4676486</v>
+        <v>4283049</v>
       </c>
       <c r="AW21" s="19">
-        <v>4283049</v>
+        <v>5263104</v>
       </c>
       <c r="AX21" s="19">
-        <v>5263104</v>
+        <v>5113387</v>
       </c>
       <c r="AY21" s="19">
-        <v>5113387</v>
+        <v>5465867</v>
       </c>
       <c r="AZ21" s="19">
-        <v>5465867</v>
+        <v>5607239</v>
       </c>
       <c r="BA21" s="19">
-        <v>5607239</v>
+        <v>5763248</v>
       </c>
       <c r="BB21" s="19">
-        <v>5763248</v>
+        <v>5974148</v>
       </c>
     </row>
     <row r="22" spans="2:54" x14ac:dyDescent="0.3">
@@ -3641,41 +3641,41 @@
       <c r="AP28" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AQ28" s="11" t="s">
-        <v>57</v>
+      <c r="AQ28" s="11">
+        <v>54</v>
       </c>
       <c r="AR28" s="11">
-        <v>54</v>
+        <v>161</v>
       </c>
       <c r="AS28" s="11">
-        <v>161</v>
+        <v>83</v>
       </c>
       <c r="AT28" s="11">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="AU28" s="11">
-        <v>0</v>
+        <v>22092</v>
       </c>
       <c r="AV28" s="11">
-        <v>22092</v>
+        <v>5361</v>
       </c>
       <c r="AW28" s="11">
-        <v>5361</v>
+        <v>6982</v>
       </c>
       <c r="AX28" s="11">
-        <v>6982</v>
+        <v>9055</v>
       </c>
       <c r="AY28" s="11">
-        <v>9055</v>
+        <v>27127</v>
       </c>
       <c r="AZ28" s="11">
-        <v>27127</v>
+        <v>67954</v>
       </c>
       <c r="BA28" s="11">
-        <v>67954</v>
+        <v>113228</v>
       </c>
       <c r="BB28" s="11">
-        <v>113228</v>
+        <v>44703</v>
       </c>
     </row>
     <row r="29" spans="2:54" x14ac:dyDescent="0.3">
@@ -3710,8 +3710,8 @@
       <c r="L29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="M29" s="13" t="s">
-        <v>57</v>
+      <c r="M29" s="13">
+        <v>0</v>
       </c>
       <c r="N29" s="13">
         <v>0</v>
@@ -3728,8 +3728,8 @@
       <c r="R29" s="13">
         <v>0</v>
       </c>
-      <c r="S29" s="13">
-        <v>0</v>
+      <c r="S29" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="T29" s="13" t="s">
         <v>57</v>
@@ -3737,35 +3737,35 @@
       <c r="U29" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="V29" s="13" t="s">
-        <v>57</v>
+      <c r="V29" s="13">
+        <v>48</v>
       </c>
       <c r="W29" s="13">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="X29" s="13">
         <v>0</v>
       </c>
       <c r="Y29" s="13">
-        <v>0</v>
+        <v>10948</v>
       </c>
       <c r="Z29" s="13">
-        <v>10948</v>
+        <v>20348</v>
       </c>
       <c r="AA29" s="13">
-        <v>20348</v>
+        <v>13698</v>
       </c>
       <c r="AB29" s="13">
-        <v>13698</v>
+        <v>2375</v>
       </c>
       <c r="AC29" s="13">
-        <v>2375</v>
+        <v>20534</v>
       </c>
       <c r="AD29" s="13">
-        <v>20534</v>
-      </c>
-      <c r="AE29" s="13">
         <v>15608</v>
+      </c>
+      <c r="AE29" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AF29" s="13" t="s">
         <v>57</v>
@@ -3846,59 +3846,59 @@
       </c>
       <c r="D30" s="11"/>
       <c r="E30" s="11">
-        <v>3036</v>
+        <v>9935</v>
       </c>
       <c r="F30" s="11">
-        <v>9935</v>
+        <v>7100</v>
       </c>
       <c r="G30" s="11">
-        <v>7100</v>
+        <v>4601</v>
       </c>
       <c r="H30" s="11">
-        <v>4601</v>
+        <v>7567</v>
       </c>
       <c r="I30" s="11">
-        <v>7567</v>
+        <v>3988</v>
       </c>
       <c r="J30" s="11">
-        <v>3988</v>
+        <v>3644</v>
       </c>
       <c r="K30" s="11">
-        <v>3644</v>
+        <v>7443</v>
       </c>
       <c r="L30" s="11">
-        <v>7443</v>
+        <v>4792</v>
       </c>
       <c r="M30" s="11">
-        <v>4792</v>
+        <v>8106</v>
       </c>
       <c r="N30" s="11">
-        <v>8106</v>
+        <v>4769</v>
       </c>
       <c r="O30" s="11">
-        <v>4769</v>
+        <v>6577</v>
       </c>
       <c r="P30" s="11">
-        <v>6577</v>
+        <v>14007</v>
       </c>
       <c r="Q30" s="11">
-        <v>14007</v>
+        <v>8143</v>
       </c>
       <c r="R30" s="11">
-        <v>8143</v>
+        <v>18203</v>
       </c>
       <c r="S30" s="11">
-        <v>18203</v>
+        <v>8036</v>
       </c>
       <c r="T30" s="11">
-        <v>8036</v>
+        <v>4592</v>
       </c>
       <c r="U30" s="11">
-        <v>4592</v>
-      </c>
-      <c r="V30" s="11">
         <v>1369</v>
       </c>
+      <c r="V30" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="W30" s="11" t="s">
         <v>57</v>
       </c>
@@ -3923,44 +3923,44 @@
       <c r="AD30" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AE30" s="11" t="s">
-        <v>57</v>
+      <c r="AE30" s="11">
+        <v>8944</v>
       </c>
       <c r="AF30" s="11">
-        <v>8944</v>
+        <v>16045</v>
       </c>
       <c r="AG30" s="11">
-        <v>16045</v>
+        <v>24535</v>
       </c>
       <c r="AH30" s="11">
-        <v>24535</v>
+        <v>12741</v>
       </c>
       <c r="AI30" s="11">
-        <v>12741</v>
+        <v>27898</v>
       </c>
       <c r="AJ30" s="11">
-        <v>27898</v>
+        <v>22200</v>
       </c>
       <c r="AK30" s="11">
-        <v>22200</v>
+        <v>18906</v>
       </c>
       <c r="AL30" s="11">
-        <v>18906</v>
+        <v>22216</v>
       </c>
       <c r="AM30" s="11">
-        <v>22216</v>
+        <v>7750</v>
       </c>
       <c r="AN30" s="11">
-        <v>7750</v>
+        <v>5959</v>
       </c>
       <c r="AO30" s="11">
-        <v>5959</v>
+        <v>1144</v>
       </c>
       <c r="AP30" s="11">
-        <v>1144</v>
-      </c>
-      <c r="AQ30" s="11">
         <v>770</v>
+      </c>
+      <c r="AQ30" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="AR30" s="11" t="s">
         <v>57</v>
@@ -4005,121 +4005,121 @@
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="13">
-        <v>1260033</v>
+        <v>1035002</v>
       </c>
       <c r="F31" s="13">
-        <v>1035002</v>
+        <v>718374</v>
       </c>
       <c r="G31" s="13">
-        <v>718374</v>
+        <v>1189492</v>
       </c>
       <c r="H31" s="13">
-        <v>1189492</v>
+        <v>1080783</v>
       </c>
       <c r="I31" s="13">
-        <v>1080783</v>
+        <v>857098</v>
       </c>
       <c r="J31" s="13">
-        <v>857098</v>
+        <v>680151</v>
       </c>
       <c r="K31" s="13">
-        <v>680151</v>
+        <v>1004705</v>
       </c>
       <c r="L31" s="13">
-        <v>1004705</v>
+        <v>581528</v>
       </c>
       <c r="M31" s="13">
-        <v>581528</v>
+        <v>521843</v>
       </c>
       <c r="N31" s="13">
-        <v>521843</v>
+        <v>704356</v>
       </c>
       <c r="O31" s="13">
-        <v>704356</v>
+        <v>1207983</v>
       </c>
       <c r="P31" s="13">
-        <v>1207983</v>
+        <v>1004666</v>
       </c>
       <c r="Q31" s="13">
-        <v>1004666</v>
+        <v>1169668</v>
       </c>
       <c r="R31" s="13">
-        <v>1169668</v>
+        <v>1216233</v>
       </c>
       <c r="S31" s="13">
-        <v>1216233</v>
+        <v>1191449</v>
       </c>
       <c r="T31" s="13">
-        <v>1191449</v>
+        <v>1291954</v>
       </c>
       <c r="U31" s="13">
-        <v>1291954</v>
+        <v>1203380</v>
       </c>
       <c r="V31" s="13">
-        <v>1203380</v>
+        <v>281680</v>
       </c>
       <c r="W31" s="13">
-        <v>281680</v>
+        <v>369371</v>
       </c>
       <c r="X31" s="13">
-        <v>369371</v>
+        <v>317221</v>
       </c>
       <c r="Y31" s="13">
-        <v>317221</v>
+        <v>533139</v>
       </c>
       <c r="Z31" s="13">
-        <v>533139</v>
+        <v>604078</v>
       </c>
       <c r="AA31" s="13">
-        <v>604078</v>
+        <v>616861</v>
       </c>
       <c r="AB31" s="13">
-        <v>616861</v>
+        <v>748073</v>
       </c>
       <c r="AC31" s="13">
-        <v>748073</v>
+        <v>818293</v>
       </c>
       <c r="AD31" s="13">
-        <v>818293</v>
+        <v>621988</v>
       </c>
       <c r="AE31" s="13">
-        <v>621988</v>
+        <v>285868</v>
       </c>
       <c r="AF31" s="13">
-        <v>285868</v>
+        <v>447174</v>
       </c>
       <c r="AG31" s="13">
-        <v>447174</v>
+        <v>473283</v>
       </c>
       <c r="AH31" s="13">
-        <v>473283</v>
+        <v>430385</v>
       </c>
       <c r="AI31" s="13">
-        <v>430385</v>
+        <v>409438</v>
       </c>
       <c r="AJ31" s="13">
-        <v>409438</v>
+        <v>434565</v>
       </c>
       <c r="AK31" s="13">
-        <v>434565</v>
+        <v>579071</v>
       </c>
       <c r="AL31" s="13">
-        <v>579071</v>
+        <v>1017576</v>
       </c>
       <c r="AM31" s="13">
-        <v>1017576</v>
+        <v>882545</v>
       </c>
       <c r="AN31" s="13">
-        <v>882545</v>
+        <v>888176</v>
       </c>
       <c r="AO31" s="13">
-        <v>888176</v>
+        <v>1743227</v>
       </c>
       <c r="AP31" s="13">
-        <v>1743227</v>
-      </c>
-      <c r="AQ31" s="13">
         <v>1426828</v>
+      </c>
+      <c r="AQ31" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AR31" s="13" t="s">
         <v>57</v>
@@ -4164,154 +4164,154 @@
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11">
-        <v>314943</v>
+        <v>396169</v>
       </c>
       <c r="F32" s="11">
-        <v>396169</v>
+        <v>306308</v>
       </c>
       <c r="G32" s="11">
-        <v>306308</v>
+        <v>306309</v>
       </c>
       <c r="H32" s="11">
-        <v>306309</v>
+        <v>397350</v>
       </c>
       <c r="I32" s="11">
-        <v>397350</v>
+        <v>378257</v>
       </c>
       <c r="J32" s="11">
-        <v>378257</v>
+        <v>292522</v>
       </c>
       <c r="K32" s="11">
-        <v>292522</v>
+        <v>483091</v>
       </c>
       <c r="L32" s="11">
-        <v>483091</v>
+        <v>328209</v>
       </c>
       <c r="M32" s="11">
-        <v>328209</v>
+        <v>404614</v>
       </c>
       <c r="N32" s="11">
-        <v>404614</v>
+        <v>418113</v>
       </c>
       <c r="O32" s="11">
-        <v>418113</v>
+        <v>348461</v>
       </c>
       <c r="P32" s="11">
-        <v>348461</v>
+        <v>556401</v>
       </c>
       <c r="Q32" s="11">
-        <v>556401</v>
+        <v>657406</v>
       </c>
       <c r="R32" s="11">
-        <v>657406</v>
+        <v>442385</v>
       </c>
       <c r="S32" s="11">
-        <v>442385</v>
+        <v>491803</v>
       </c>
       <c r="T32" s="11">
-        <v>491803</v>
+        <v>492971</v>
       </c>
       <c r="U32" s="11">
-        <v>492971</v>
+        <v>415549</v>
       </c>
       <c r="V32" s="11">
-        <v>415549</v>
+        <v>228277</v>
       </c>
       <c r="W32" s="11">
-        <v>228277</v>
+        <v>435893</v>
       </c>
       <c r="X32" s="11">
-        <v>435893</v>
+        <v>461868</v>
       </c>
       <c r="Y32" s="11">
-        <v>461868</v>
+        <v>524087</v>
       </c>
       <c r="Z32" s="11">
-        <v>524087</v>
+        <v>569274</v>
       </c>
       <c r="AA32" s="11">
-        <v>569274</v>
+        <v>469036</v>
       </c>
       <c r="AB32" s="11">
-        <v>469036</v>
+        <v>580123</v>
       </c>
       <c r="AC32" s="11">
-        <v>580123</v>
+        <v>546227</v>
       </c>
       <c r="AD32" s="11">
-        <v>546227</v>
+        <v>484651</v>
       </c>
       <c r="AE32" s="11">
-        <v>484651</v>
+        <v>467528</v>
       </c>
       <c r="AF32" s="11">
-        <v>467528</v>
+        <v>587126</v>
       </c>
       <c r="AG32" s="11">
-        <v>587126</v>
+        <v>618410</v>
       </c>
       <c r="AH32" s="11">
-        <v>618410</v>
+        <v>290689</v>
       </c>
       <c r="AI32" s="11">
-        <v>290689</v>
+        <v>604996</v>
       </c>
       <c r="AJ32" s="11">
-        <v>604996</v>
+        <v>597149</v>
       </c>
       <c r="AK32" s="11">
-        <v>597149</v>
+        <v>624677</v>
       </c>
       <c r="AL32" s="11">
-        <v>624677</v>
+        <v>592899</v>
       </c>
       <c r="AM32" s="11">
-        <v>592899</v>
+        <v>1180222</v>
       </c>
       <c r="AN32" s="11">
-        <v>1180222</v>
+        <v>484775</v>
       </c>
       <c r="AO32" s="11">
-        <v>484775</v>
+        <v>660278</v>
       </c>
       <c r="AP32" s="11">
-        <v>660278</v>
+        <v>654112</v>
       </c>
       <c r="AQ32" s="11">
-        <v>654112</v>
+        <v>549674</v>
       </c>
       <c r="AR32" s="11">
-        <v>549674</v>
+        <v>770343</v>
       </c>
       <c r="AS32" s="11">
-        <v>770343</v>
+        <v>584600</v>
       </c>
       <c r="AT32" s="11">
-        <v>584600</v>
+        <v>505100</v>
       </c>
       <c r="AU32" s="11">
-        <v>505100</v>
+        <v>764278</v>
       </c>
       <c r="AV32" s="11">
-        <v>764278</v>
+        <v>652335</v>
       </c>
       <c r="AW32" s="11">
-        <v>652335</v>
+        <v>800196</v>
       </c>
       <c r="AX32" s="11">
-        <v>800196</v>
+        <v>604770</v>
       </c>
       <c r="AY32" s="11">
-        <v>604770</v>
+        <v>599261</v>
       </c>
       <c r="AZ32" s="11">
-        <v>599261</v>
+        <v>818718</v>
       </c>
       <c r="BA32" s="11">
-        <v>818718</v>
+        <v>591590</v>
       </c>
       <c r="BB32" s="11">
-        <v>591590</v>
+        <v>670271</v>
       </c>
     </row>
     <row r="33" spans="2:54" x14ac:dyDescent="0.3">
@@ -4323,154 +4323,154 @@
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="13">
-        <v>1586972</v>
+        <v>1527485</v>
       </c>
       <c r="F33" s="13">
-        <v>1527485</v>
+        <v>1702213</v>
       </c>
       <c r="G33" s="13">
-        <v>1702213</v>
+        <v>1654419</v>
       </c>
       <c r="H33" s="13">
-        <v>1654419</v>
+        <v>1273669</v>
       </c>
       <c r="I33" s="13">
-        <v>1273669</v>
+        <v>1161172</v>
       </c>
       <c r="J33" s="13">
-        <v>1161172</v>
+        <v>716577</v>
       </c>
       <c r="K33" s="13">
-        <v>716577</v>
+        <v>1458147</v>
       </c>
       <c r="L33" s="13">
-        <v>1458147</v>
+        <v>1006140</v>
       </c>
       <c r="M33" s="13">
-        <v>1006140</v>
+        <v>1119795</v>
       </c>
       <c r="N33" s="13">
-        <v>1119795</v>
+        <v>1177604</v>
       </c>
       <c r="O33" s="13">
-        <v>1177604</v>
+        <v>2131309</v>
       </c>
       <c r="P33" s="13">
-        <v>2131309</v>
+        <v>1486376</v>
       </c>
       <c r="Q33" s="13">
-        <v>1486376</v>
+        <v>1999666</v>
       </c>
       <c r="R33" s="13">
-        <v>1999666</v>
+        <v>1897971</v>
       </c>
       <c r="S33" s="13">
-        <v>1897971</v>
+        <v>1970630</v>
       </c>
       <c r="T33" s="13">
-        <v>1970630</v>
+        <v>1626291</v>
       </c>
       <c r="U33" s="13">
-        <v>1626291</v>
+        <v>1704305</v>
       </c>
       <c r="V33" s="13">
-        <v>1704305</v>
+        <v>865575</v>
       </c>
       <c r="W33" s="13">
-        <v>865575</v>
+        <v>1667938</v>
       </c>
       <c r="X33" s="13">
-        <v>1667938</v>
+        <v>1385208</v>
       </c>
       <c r="Y33" s="13">
-        <v>1385208</v>
+        <v>1638157</v>
       </c>
       <c r="Z33" s="13">
-        <v>1638157</v>
+        <v>1745177</v>
       </c>
       <c r="AA33" s="13">
-        <v>1745177</v>
+        <v>3054737</v>
       </c>
       <c r="AB33" s="13">
-        <v>3054737</v>
+        <v>2065738</v>
       </c>
       <c r="AC33" s="13">
-        <v>2065738</v>
+        <v>1916090</v>
       </c>
       <c r="AD33" s="13">
-        <v>1916090</v>
+        <v>1853922</v>
       </c>
       <c r="AE33" s="13">
-        <v>1853922</v>
+        <v>1098306</v>
       </c>
       <c r="AF33" s="13">
-        <v>1098306</v>
+        <v>1325890</v>
       </c>
       <c r="AG33" s="13">
-        <v>1325890</v>
+        <v>1484449</v>
       </c>
       <c r="AH33" s="13">
-        <v>1484449</v>
+        <v>878485</v>
       </c>
       <c r="AI33" s="13">
-        <v>878485</v>
+        <v>1373375</v>
       </c>
       <c r="AJ33" s="13">
-        <v>1373375</v>
+        <v>1241736</v>
       </c>
       <c r="AK33" s="13">
-        <v>1241736</v>
+        <v>1725798</v>
       </c>
       <c r="AL33" s="13">
-        <v>1725798</v>
+        <v>2041833</v>
       </c>
       <c r="AM33" s="13">
-        <v>2041833</v>
+        <v>2496537</v>
       </c>
       <c r="AN33" s="13">
-        <v>2496537</v>
+        <v>1915831</v>
       </c>
       <c r="AO33" s="13">
-        <v>1915831</v>
+        <v>2466074</v>
       </c>
       <c r="AP33" s="13">
-        <v>2466074</v>
+        <v>2349339</v>
       </c>
       <c r="AQ33" s="13">
-        <v>2349339</v>
+        <v>2161640</v>
       </c>
       <c r="AR33" s="13">
-        <v>2161640</v>
+        <v>3298955</v>
       </c>
       <c r="AS33" s="13">
-        <v>3298955</v>
+        <v>2668062</v>
       </c>
       <c r="AT33" s="13">
-        <v>2668062</v>
+        <v>1737915</v>
       </c>
       <c r="AU33" s="13">
-        <v>1737915</v>
+        <v>2369428</v>
       </c>
       <c r="AV33" s="13">
-        <v>2369428</v>
+        <v>2318179</v>
       </c>
       <c r="AW33" s="13">
-        <v>2318179</v>
+        <v>2353065</v>
       </c>
       <c r="AX33" s="13">
-        <v>2353065</v>
+        <v>2319043</v>
       </c>
       <c r="AY33" s="13">
-        <v>2319043</v>
+        <v>2644829</v>
       </c>
       <c r="AZ33" s="13">
-        <v>2644829</v>
+        <v>3332828</v>
       </c>
       <c r="BA33" s="13">
-        <v>3332828</v>
+        <v>3208570</v>
       </c>
       <c r="BB33" s="13">
-        <v>3208570</v>
+        <v>2778600</v>
       </c>
     </row>
     <row r="34" spans="2:54" x14ac:dyDescent="0.3">
@@ -4487,11 +4487,11 @@
       <c r="F34" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G34" s="11" t="s">
-        <v>57</v>
+      <c r="G34" s="11">
+        <v>82</v>
       </c>
       <c r="H34" s="11">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I34" s="11">
         <v>0</v>
@@ -4523,8 +4523,8 @@
       <c r="R34" s="11">
         <v>0</v>
       </c>
-      <c r="S34" s="11">
-        <v>0</v>
+      <c r="S34" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="T34" s="11" t="s">
         <v>57</v>
@@ -4754,41 +4754,41 @@
       <c r="AP35" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AQ35" s="13" t="s">
-        <v>57</v>
+      <c r="AQ35" s="13">
+        <v>1420484</v>
       </c>
       <c r="AR35" s="13">
-        <v>1420484</v>
+        <v>2038343</v>
       </c>
       <c r="AS35" s="13">
-        <v>2038343</v>
+        <v>877845</v>
       </c>
       <c r="AT35" s="13">
-        <v>877845</v>
+        <v>1173513</v>
       </c>
       <c r="AU35" s="13">
-        <v>1173513</v>
+        <v>1932014</v>
       </c>
       <c r="AV35" s="13">
-        <v>1932014</v>
+        <v>1301217</v>
       </c>
       <c r="AW35" s="13">
-        <v>1301217</v>
+        <v>1254593</v>
       </c>
       <c r="AX35" s="13">
-        <v>1254593</v>
+        <v>1141767</v>
       </c>
       <c r="AY35" s="13">
-        <v>1141767</v>
+        <v>1155716</v>
       </c>
       <c r="AZ35" s="13">
-        <v>1155716</v>
+        <v>2570354</v>
       </c>
       <c r="BA35" s="13">
-        <v>2570354</v>
+        <v>2499780</v>
       </c>
       <c r="BB35" s="13">
-        <v>2499780</v>
+        <v>1954756</v>
       </c>
     </row>
     <row r="36" spans="2:54" x14ac:dyDescent="0.3">
@@ -4932,8 +4932,8 @@
       <c r="AD37" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AE37" s="17" t="s">
-        <v>57</v>
+      <c r="AE37" s="17">
+        <v>0</v>
       </c>
       <c r="AF37" s="17">
         <v>0</v>
@@ -5146,8 +5146,8 @@
       <c r="AD39" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AE39" s="17" t="s">
-        <v>57</v>
+      <c r="AE39" s="17">
+        <v>0</v>
       </c>
       <c r="AF39" s="17">
         <v>0</v>
@@ -5226,154 +5226,154 @@
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19">
-        <v>3164984</v>
+        <v>2968591</v>
       </c>
       <c r="F40" s="19">
-        <v>2968591</v>
+        <v>2733995</v>
       </c>
       <c r="G40" s="19">
-        <v>2733995</v>
+        <v>3154903</v>
       </c>
       <c r="H40" s="19">
-        <v>3154903</v>
+        <v>2759369</v>
       </c>
       <c r="I40" s="19">
-        <v>2759369</v>
+        <v>2400515</v>
       </c>
       <c r="J40" s="19">
-        <v>2400515</v>
+        <v>1692894</v>
       </c>
       <c r="K40" s="19">
-        <v>1692894</v>
+        <v>2953386</v>
       </c>
       <c r="L40" s="19">
-        <v>2953386</v>
+        <v>1920669</v>
       </c>
       <c r="M40" s="19">
-        <v>1920669</v>
+        <v>2054358</v>
       </c>
       <c r="N40" s="19">
-        <v>2054358</v>
+        <v>2304842</v>
       </c>
       <c r="O40" s="19">
-        <v>2304842</v>
+        <v>3694330</v>
       </c>
       <c r="P40" s="19">
-        <v>3694330</v>
+        <v>3061450</v>
       </c>
       <c r="Q40" s="19">
-        <v>3061450</v>
+        <v>3834883</v>
       </c>
       <c r="R40" s="19">
-        <v>3834883</v>
+        <v>3574792</v>
       </c>
       <c r="S40" s="19">
-        <v>3574792</v>
+        <v>3661918</v>
       </c>
       <c r="T40" s="19">
-        <v>3661918</v>
+        <v>3415808</v>
       </c>
       <c r="U40" s="19">
-        <v>3415808</v>
+        <v>3324603</v>
       </c>
       <c r="V40" s="19">
-        <v>3324603</v>
+        <v>1375580</v>
       </c>
       <c r="W40" s="19">
-        <v>1375580</v>
+        <v>2473202</v>
       </c>
       <c r="X40" s="19">
-        <v>2473202</v>
+        <v>2164297</v>
       </c>
       <c r="Y40" s="19">
-        <v>2164297</v>
+        <v>2706331</v>
       </c>
       <c r="Z40" s="19">
-        <v>2706331</v>
+        <v>2938877</v>
       </c>
       <c r="AA40" s="19">
-        <v>2938877</v>
+        <v>4154332</v>
       </c>
       <c r="AB40" s="19">
-        <v>4154332</v>
+        <v>3396309</v>
       </c>
       <c r="AC40" s="19">
-        <v>3396309</v>
+        <v>3301144</v>
       </c>
       <c r="AD40" s="19">
-        <v>3301144</v>
+        <v>2976169</v>
       </c>
       <c r="AE40" s="19">
-        <v>2976169</v>
+        <v>1860646</v>
       </c>
       <c r="AF40" s="19">
-        <v>1860646</v>
+        <v>2376235</v>
       </c>
       <c r="AG40" s="19">
-        <v>2376235</v>
+        <v>2600677</v>
       </c>
       <c r="AH40" s="19">
-        <v>2600677</v>
+        <v>1612300</v>
       </c>
       <c r="AI40" s="19">
-        <v>1612300</v>
+        <v>2415707</v>
       </c>
       <c r="AJ40" s="19">
-        <v>2415707</v>
+        <v>2295650</v>
       </c>
       <c r="AK40" s="19">
-        <v>2295650</v>
+        <v>2948452</v>
       </c>
       <c r="AL40" s="19">
-        <v>2948452</v>
+        <v>3674524</v>
       </c>
       <c r="AM40" s="19">
-        <v>3674524</v>
+        <v>4567054</v>
       </c>
       <c r="AN40" s="19">
-        <v>4567054</v>
+        <v>3294741</v>
       </c>
       <c r="AO40" s="19">
-        <v>3294741</v>
+        <v>4870723</v>
       </c>
       <c r="AP40" s="19">
-        <v>4870723</v>
+        <v>4431049</v>
       </c>
       <c r="AQ40" s="19">
-        <v>4431049</v>
+        <v>4131852</v>
       </c>
       <c r="AR40" s="19">
-        <v>4131852</v>
+        <v>6107802</v>
       </c>
       <c r="AS40" s="19">
-        <v>6107802</v>
+        <v>4130590</v>
       </c>
       <c r="AT40" s="19">
-        <v>4130590</v>
+        <v>3416528</v>
       </c>
       <c r="AU40" s="19">
-        <v>3416528</v>
+        <v>5087812</v>
       </c>
       <c r="AV40" s="19">
-        <v>5087812</v>
+        <v>4277092</v>
       </c>
       <c r="AW40" s="19">
-        <v>4277092</v>
+        <v>4414836</v>
       </c>
       <c r="AX40" s="19">
-        <v>4414836</v>
+        <v>4074635</v>
       </c>
       <c r="AY40" s="19">
-        <v>4074635</v>
+        <v>4426933</v>
       </c>
       <c r="AZ40" s="19">
-        <v>4426933</v>
+        <v>6789854</v>
       </c>
       <c r="BA40" s="19">
-        <v>6789854</v>
+        <v>6413168</v>
       </c>
       <c r="BB40" s="19">
-        <v>6413168</v>
+        <v>5448330</v>
       </c>
     </row>
     <row r="41" spans="2:54" x14ac:dyDescent="0.3">
@@ -5932,41 +5932,41 @@
       <c r="AP47" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AQ47" s="11" t="s">
-        <v>57</v>
+      <c r="AQ47" s="11">
+        <v>33</v>
       </c>
       <c r="AR47" s="11">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="AS47" s="11">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="AT47" s="11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AU47" s="11">
-        <v>0</v>
+        <v>13969</v>
       </c>
       <c r="AV47" s="11">
-        <v>13969</v>
+        <v>3389</v>
       </c>
       <c r="AW47" s="11">
-        <v>3389</v>
+        <v>4415</v>
       </c>
       <c r="AX47" s="11">
-        <v>4415</v>
+        <v>5727</v>
       </c>
       <c r="AY47" s="11">
-        <v>5727</v>
+        <v>42971</v>
       </c>
       <c r="AZ47" s="11">
-        <v>42971</v>
+        <v>47899</v>
       </c>
       <c r="BA47" s="11">
-        <v>47899</v>
+        <v>64866</v>
       </c>
       <c r="BB47" s="11">
-        <v>64866</v>
+        <v>45500</v>
       </c>
     </row>
     <row r="48" spans="2:54" x14ac:dyDescent="0.3">
@@ -6001,8 +6001,8 @@
       <c r="L48" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="M48" s="13" t="s">
-        <v>57</v>
+      <c r="M48" s="13">
+        <v>0</v>
       </c>
       <c r="N48" s="13">
         <v>0</v>
@@ -6019,8 +6019,8 @@
       <c r="R48" s="13">
         <v>0</v>
       </c>
-      <c r="S48" s="13">
-        <v>0</v>
+      <c r="S48" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="T48" s="13" t="s">
         <v>57</v>
@@ -6028,35 +6028,35 @@
       <c r="U48" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="V48" s="13" t="s">
-        <v>57</v>
+      <c r="V48" s="13">
+        <v>29</v>
       </c>
       <c r="W48" s="13">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="X48" s="13">
         <v>0</v>
       </c>
       <c r="Y48" s="13">
-        <v>0</v>
+        <v>6647</v>
       </c>
       <c r="Z48" s="13">
-        <v>6647</v>
+        <v>12369</v>
       </c>
       <c r="AA48" s="13">
-        <v>12369</v>
+        <v>8260</v>
       </c>
       <c r="AB48" s="13">
-        <v>8260</v>
+        <v>1414</v>
       </c>
       <c r="AC48" s="13">
-        <v>1414</v>
+        <v>11085</v>
       </c>
       <c r="AD48" s="13">
-        <v>11085</v>
-      </c>
-      <c r="AE48" s="13">
         <v>9420</v>
+      </c>
+      <c r="AE48" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AF48" s="13" t="s">
         <v>57</v>
@@ -6137,59 +6137,59 @@
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11">
-        <v>2310</v>
+        <v>7866</v>
       </c>
       <c r="F49" s="11">
-        <v>7866</v>
+        <v>5526</v>
       </c>
       <c r="G49" s="11">
-        <v>5526</v>
+        <v>3661</v>
       </c>
       <c r="H49" s="11">
-        <v>3661</v>
+        <v>6008</v>
       </c>
       <c r="I49" s="11">
-        <v>6008</v>
+        <v>2748</v>
       </c>
       <c r="J49" s="11">
-        <v>2748</v>
+        <v>2935</v>
       </c>
       <c r="K49" s="11">
-        <v>2935</v>
+        <v>5969</v>
       </c>
       <c r="L49" s="11">
-        <v>5969</v>
+        <v>3828</v>
       </c>
       <c r="M49" s="11">
-        <v>3828</v>
+        <v>6522</v>
       </c>
       <c r="N49" s="11">
-        <v>6522</v>
+        <v>2927</v>
       </c>
       <c r="O49" s="11">
-        <v>2927</v>
+        <v>4002</v>
       </c>
       <c r="P49" s="11">
-        <v>4002</v>
+        <v>7827</v>
       </c>
       <c r="Q49" s="11">
-        <v>7827</v>
+        <v>4573</v>
       </c>
       <c r="R49" s="11">
-        <v>4573</v>
+        <v>10634</v>
       </c>
       <c r="S49" s="11">
-        <v>10634</v>
+        <v>4593</v>
       </c>
       <c r="T49" s="11">
-        <v>4593</v>
+        <v>2730</v>
       </c>
       <c r="U49" s="11">
-        <v>2730</v>
-      </c>
-      <c r="V49" s="11">
         <v>811</v>
       </c>
+      <c r="V49" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="W49" s="11" t="s">
         <v>57</v>
       </c>
@@ -6214,44 +6214,44 @@
       <c r="AD49" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AE49" s="11" t="s">
-        <v>57</v>
+      <c r="AE49" s="11">
+        <v>5389</v>
       </c>
       <c r="AF49" s="11">
-        <v>5389</v>
+        <v>8694</v>
       </c>
       <c r="AG49" s="11">
-        <v>8694</v>
+        <v>13955</v>
       </c>
       <c r="AH49" s="11">
-        <v>13955</v>
+        <v>7385</v>
       </c>
       <c r="AI49" s="11">
-        <v>7385</v>
+        <v>17172</v>
       </c>
       <c r="AJ49" s="11">
-        <v>17172</v>
+        <v>13441</v>
       </c>
       <c r="AK49" s="11">
-        <v>13441</v>
+        <v>10344</v>
       </c>
       <c r="AL49" s="11">
-        <v>10344</v>
+        <v>13415</v>
       </c>
       <c r="AM49" s="11">
-        <v>13415</v>
+        <v>4688</v>
       </c>
       <c r="AN49" s="11">
-        <v>4688</v>
+        <v>3386</v>
       </c>
       <c r="AO49" s="11">
-        <v>3386</v>
+        <v>688</v>
       </c>
       <c r="AP49" s="11">
-        <v>688</v>
-      </c>
-      <c r="AQ49" s="11">
         <v>465</v>
+      </c>
+      <c r="AQ49" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="AR49" s="11" t="s">
         <v>57</v>
@@ -6296,121 +6296,121 @@
       </c>
       <c r="D50" s="13"/>
       <c r="E50" s="13">
-        <v>44366</v>
+        <v>34650</v>
       </c>
       <c r="F50" s="13">
-        <v>34650</v>
+        <v>24627</v>
       </c>
       <c r="G50" s="13">
-        <v>24627</v>
+        <v>45233</v>
       </c>
       <c r="H50" s="13">
-        <v>45233</v>
+        <v>46583</v>
       </c>
       <c r="I50" s="13">
-        <v>46583</v>
+        <v>34764</v>
       </c>
       <c r="J50" s="13">
-        <v>34764</v>
+        <v>35419</v>
       </c>
       <c r="K50" s="13">
-        <v>35419</v>
+        <v>44956</v>
       </c>
       <c r="L50" s="13">
-        <v>44956</v>
+        <v>31684</v>
       </c>
       <c r="M50" s="13">
-        <v>31684</v>
+        <v>26724</v>
       </c>
       <c r="N50" s="13">
-        <v>26724</v>
+        <v>39414</v>
       </c>
       <c r="O50" s="13">
-        <v>39414</v>
+        <v>66525</v>
       </c>
       <c r="P50" s="13">
-        <v>66525</v>
+        <v>62519</v>
       </c>
       <c r="Q50" s="13">
-        <v>62519</v>
+        <v>69485</v>
       </c>
       <c r="R50" s="13">
-        <v>69485</v>
+        <v>83915</v>
       </c>
       <c r="S50" s="13">
-        <v>83915</v>
+        <v>70279</v>
       </c>
       <c r="T50" s="13">
-        <v>70279</v>
+        <v>79786</v>
       </c>
       <c r="U50" s="13">
-        <v>79786</v>
+        <v>79165</v>
       </c>
       <c r="V50" s="13">
-        <v>79165</v>
+        <v>18129</v>
       </c>
       <c r="W50" s="13">
-        <v>18129</v>
+        <v>23161</v>
       </c>
       <c r="X50" s="13">
-        <v>23161</v>
+        <v>20186</v>
       </c>
       <c r="Y50" s="13">
-        <v>20186</v>
+        <v>32626</v>
       </c>
       <c r="Z50" s="13">
-        <v>32626</v>
+        <v>38436</v>
       </c>
       <c r="AA50" s="13">
-        <v>38436</v>
+        <v>54774</v>
       </c>
       <c r="AB50" s="13">
-        <v>54774</v>
+        <v>65731</v>
       </c>
       <c r="AC50" s="13">
-        <v>65731</v>
+        <v>87502</v>
       </c>
       <c r="AD50" s="13">
-        <v>87502</v>
+        <v>54737</v>
       </c>
       <c r="AE50" s="13">
-        <v>54737</v>
+        <v>25987</v>
       </c>
       <c r="AF50" s="13">
-        <v>25987</v>
+        <v>36320</v>
       </c>
       <c r="AG50" s="13">
-        <v>36320</v>
+        <v>40514</v>
       </c>
       <c r="AH50" s="13">
-        <v>40514</v>
+        <v>41747</v>
       </c>
       <c r="AI50" s="13">
-        <v>41747</v>
+        <v>36246</v>
       </c>
       <c r="AJ50" s="13">
-        <v>36246</v>
+        <v>38689</v>
       </c>
       <c r="AK50" s="13">
-        <v>38689</v>
+        <v>50779</v>
       </c>
       <c r="AL50" s="13">
-        <v>50779</v>
+        <v>85271</v>
       </c>
       <c r="AM50" s="13">
-        <v>85271</v>
+        <v>81231</v>
       </c>
       <c r="AN50" s="13">
-        <v>81231</v>
+        <v>83171</v>
       </c>
       <c r="AO50" s="13">
-        <v>83171</v>
+        <v>164100</v>
       </c>
       <c r="AP50" s="13">
-        <v>164100</v>
-      </c>
-      <c r="AQ50" s="13">
         <v>137311</v>
+      </c>
+      <c r="AQ50" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AR50" s="13" t="s">
         <v>57</v>
@@ -6455,154 +6455,154 @@
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11">
-        <v>108059</v>
+        <v>114411</v>
       </c>
       <c r="F51" s="11">
-        <v>114411</v>
+        <v>111425</v>
       </c>
       <c r="G51" s="11">
-        <v>111425</v>
+        <v>96472</v>
       </c>
       <c r="H51" s="11">
-        <v>96472</v>
+        <v>142333</v>
       </c>
       <c r="I51" s="11">
-        <v>142333</v>
+        <v>140310</v>
       </c>
       <c r="J51" s="11">
-        <v>140310</v>
+        <v>118149</v>
       </c>
       <c r="K51" s="11">
-        <v>118149</v>
+        <v>175752</v>
       </c>
       <c r="L51" s="11">
-        <v>175752</v>
+        <v>136322</v>
       </c>
       <c r="M51" s="11">
-        <v>136322</v>
+        <v>162027</v>
       </c>
       <c r="N51" s="11">
-        <v>162027</v>
+        <v>158151</v>
       </c>
       <c r="O51" s="11">
-        <v>158151</v>
+        <v>156849</v>
       </c>
       <c r="P51" s="11">
-        <v>156849</v>
+        <v>184736</v>
       </c>
       <c r="Q51" s="11">
-        <v>184736</v>
+        <v>177062</v>
       </c>
       <c r="R51" s="11">
-        <v>177062</v>
+        <v>160781</v>
       </c>
       <c r="S51" s="11">
-        <v>160781</v>
+        <v>171514</v>
       </c>
       <c r="T51" s="11">
-        <v>171514</v>
+        <v>179600</v>
       </c>
       <c r="U51" s="11">
-        <v>179600</v>
+        <v>169595</v>
       </c>
       <c r="V51" s="11">
-        <v>169595</v>
+        <v>96458</v>
       </c>
       <c r="W51" s="11">
-        <v>96458</v>
+        <v>171801</v>
       </c>
       <c r="X51" s="11">
-        <v>171801</v>
+        <v>198305</v>
       </c>
       <c r="Y51" s="11">
-        <v>198305</v>
+        <v>206039</v>
       </c>
       <c r="Z51" s="11">
-        <v>206039</v>
+        <v>241521</v>
       </c>
       <c r="AA51" s="11">
-        <v>241521</v>
+        <v>218444</v>
       </c>
       <c r="AB51" s="11">
-        <v>218444</v>
+        <v>246515</v>
       </c>
       <c r="AC51" s="11">
-        <v>246515</v>
+        <v>243601</v>
       </c>
       <c r="AD51" s="11">
-        <v>243601</v>
+        <v>244810</v>
       </c>
       <c r="AE51" s="11">
-        <v>244810</v>
+        <v>274190</v>
       </c>
       <c r="AF51" s="11">
-        <v>274190</v>
+        <v>379034</v>
       </c>
       <c r="AG51" s="11">
-        <v>379034</v>
+        <v>439931</v>
       </c>
       <c r="AH51" s="11">
-        <v>439931</v>
+        <v>214203</v>
       </c>
       <c r="AI51" s="11">
-        <v>214203</v>
+        <v>396696</v>
       </c>
       <c r="AJ51" s="11">
-        <v>396696</v>
+        <v>421257</v>
       </c>
       <c r="AK51" s="11">
-        <v>421257</v>
+        <v>415051</v>
       </c>
       <c r="AL51" s="11">
-        <v>415051</v>
+        <v>439408</v>
       </c>
       <c r="AM51" s="11">
-        <v>439408</v>
+        <v>649542</v>
       </c>
       <c r="AN51" s="11">
-        <v>649542</v>
+        <v>373516</v>
       </c>
       <c r="AO51" s="11">
-        <v>373516</v>
+        <v>534911</v>
       </c>
       <c r="AP51" s="11">
-        <v>534911</v>
+        <v>558831</v>
       </c>
       <c r="AQ51" s="11">
-        <v>558831</v>
+        <v>423922</v>
       </c>
       <c r="AR51" s="11">
-        <v>423922</v>
+        <v>522057</v>
       </c>
       <c r="AS51" s="11">
-        <v>522057</v>
+        <v>458559</v>
       </c>
       <c r="AT51" s="11">
-        <v>458559</v>
+        <v>506818</v>
       </c>
       <c r="AU51" s="11">
-        <v>506818</v>
+        <v>607517</v>
       </c>
       <c r="AV51" s="11">
-        <v>607517</v>
+        <v>675667</v>
       </c>
       <c r="AW51" s="11">
-        <v>675667</v>
+        <v>757268</v>
       </c>
       <c r="AX51" s="11">
-        <v>757268</v>
+        <v>656929</v>
       </c>
       <c r="AY51" s="11">
-        <v>656929</v>
+        <v>771724</v>
       </c>
       <c r="AZ51" s="11">
-        <v>771724</v>
+        <v>656597</v>
       </c>
       <c r="BA51" s="11">
-        <v>656597</v>
+        <v>705381</v>
       </c>
       <c r="BB51" s="11">
-        <v>705381</v>
+        <v>824204</v>
       </c>
     </row>
     <row r="52" spans="2:54" x14ac:dyDescent="0.3">
@@ -6614,154 +6614,154 @@
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="13">
-        <v>414968</v>
+        <v>443904</v>
       </c>
       <c r="F52" s="13">
-        <v>443904</v>
+        <v>395772</v>
       </c>
       <c r="G52" s="13">
-        <v>395772</v>
+        <v>431753</v>
       </c>
       <c r="H52" s="13">
-        <v>431753</v>
+        <v>469770</v>
       </c>
       <c r="I52" s="13">
-        <v>469770</v>
+        <v>537572</v>
       </c>
       <c r="J52" s="13">
-        <v>537572</v>
+        <v>319261</v>
       </c>
       <c r="K52" s="13">
-        <v>319261</v>
+        <v>631652</v>
       </c>
       <c r="L52" s="13">
-        <v>631652</v>
+        <v>500784</v>
       </c>
       <c r="M52" s="13">
-        <v>500784</v>
+        <v>584636</v>
       </c>
       <c r="N52" s="13">
-        <v>584636</v>
+        <v>539988</v>
       </c>
       <c r="O52" s="13">
-        <v>539988</v>
+        <v>648171</v>
       </c>
       <c r="P52" s="13">
-        <v>648171</v>
+        <v>746277</v>
       </c>
       <c r="Q52" s="13">
-        <v>746277</v>
+        <v>677722</v>
       </c>
       <c r="R52" s="13">
-        <v>677722</v>
+        <v>846580</v>
       </c>
       <c r="S52" s="13">
-        <v>846580</v>
+        <v>815515</v>
       </c>
       <c r="T52" s="13">
-        <v>815515</v>
+        <v>858380</v>
       </c>
       <c r="U52" s="13">
-        <v>858380</v>
+        <v>925834</v>
       </c>
       <c r="V52" s="13">
-        <v>925834</v>
+        <v>482278</v>
       </c>
       <c r="W52" s="13">
-        <v>482278</v>
+        <v>859964</v>
       </c>
       <c r="X52" s="13">
-        <v>859964</v>
+        <v>800104</v>
       </c>
       <c r="Y52" s="13">
-        <v>800104</v>
+        <v>946732</v>
       </c>
       <c r="Z52" s="13">
-        <v>946732</v>
+        <v>1015628</v>
       </c>
       <c r="AA52" s="13">
-        <v>1015628</v>
+        <v>1162426</v>
       </c>
       <c r="AB52" s="13">
-        <v>1162426</v>
+        <v>1319263</v>
       </c>
       <c r="AC52" s="13">
-        <v>1319263</v>
+        <v>1318417</v>
       </c>
       <c r="AD52" s="13">
-        <v>1318417</v>
+        <v>1208696</v>
       </c>
       <c r="AE52" s="13">
-        <v>1208696</v>
+        <v>932647</v>
       </c>
       <c r="AF52" s="13">
-        <v>932647</v>
+        <v>1079537</v>
       </c>
       <c r="AG52" s="13">
-        <v>1079537</v>
+        <v>1306898</v>
       </c>
       <c r="AH52" s="13">
-        <v>1306898</v>
+        <v>836905</v>
       </c>
       <c r="AI52" s="13">
-        <v>836905</v>
+        <v>1245568</v>
       </c>
       <c r="AJ52" s="13">
-        <v>1245568</v>
+        <v>1210612</v>
       </c>
       <c r="AK52" s="13">
-        <v>1210612</v>
+        <v>1432926</v>
       </c>
       <c r="AL52" s="13">
-        <v>1432926</v>
+        <v>1648490</v>
       </c>
       <c r="AM52" s="13">
-        <v>1648490</v>
+        <v>2071678</v>
       </c>
       <c r="AN52" s="13">
-        <v>2071678</v>
+        <v>1684209</v>
       </c>
       <c r="AO52" s="13">
-        <v>1684209</v>
+        <v>1943942</v>
       </c>
       <c r="AP52" s="13">
-        <v>1943942</v>
+        <v>2148252</v>
       </c>
       <c r="AQ52" s="13">
-        <v>2148252</v>
+        <v>1762613</v>
       </c>
       <c r="AR52" s="13">
-        <v>1762613</v>
+        <v>2377872</v>
       </c>
       <c r="AS52" s="13">
-        <v>2377872</v>
+        <v>2238813</v>
       </c>
       <c r="AT52" s="13">
-        <v>2238813</v>
+        <v>1694191</v>
       </c>
       <c r="AU52" s="13">
-        <v>1694191</v>
+        <v>2442669</v>
       </c>
       <c r="AV52" s="13">
-        <v>2442669</v>
+        <v>2469638</v>
       </c>
       <c r="AW52" s="13">
-        <v>2469638</v>
+        <v>2589891</v>
       </c>
       <c r="AX52" s="13">
-        <v>2589891</v>
+        <v>3462720</v>
       </c>
       <c r="AY52" s="13">
-        <v>3462720</v>
+        <v>3786997</v>
       </c>
       <c r="AZ52" s="13">
-        <v>3786997</v>
+        <v>4341185</v>
       </c>
       <c r="BA52" s="13">
-        <v>4341185</v>
+        <v>4881214</v>
       </c>
       <c r="BB52" s="13">
-        <v>4881214</v>
+        <v>4660790</v>
       </c>
     </row>
     <row r="53" spans="2:54" x14ac:dyDescent="0.3">
@@ -6778,11 +6778,11 @@
       <c r="F53" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G53" s="11" t="s">
-        <v>57</v>
+      <c r="G53" s="11">
+        <v>1</v>
       </c>
       <c r="H53" s="11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" s="11">
         <v>0</v>
@@ -6814,8 +6814,8 @@
       <c r="R53" s="11">
         <v>0</v>
       </c>
-      <c r="S53" s="11">
-        <v>0</v>
+      <c r="S53" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="T53" s="11" t="s">
         <v>57</v>
@@ -7045,41 +7045,41 @@
       <c r="AP54" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AQ54" s="13" t="s">
-        <v>57</v>
+      <c r="AQ54" s="13">
+        <v>132301</v>
       </c>
       <c r="AR54" s="13">
-        <v>132301</v>
+        <v>200459</v>
       </c>
       <c r="AS54" s="13">
-        <v>200459</v>
+        <v>91826</v>
       </c>
       <c r="AT54" s="13">
-        <v>91826</v>
+        <v>145401</v>
       </c>
       <c r="AU54" s="13">
-        <v>145401</v>
+        <v>237817</v>
       </c>
       <c r="AV54" s="13">
-        <v>237817</v>
+        <v>162979</v>
       </c>
       <c r="AW54" s="13">
-        <v>162979</v>
+        <v>160563</v>
       </c>
       <c r="AX54" s="13">
-        <v>160563</v>
+        <v>154226</v>
       </c>
       <c r="AY54" s="13">
-        <v>154226</v>
+        <v>153366</v>
       </c>
       <c r="AZ54" s="13">
-        <v>153366</v>
+        <v>339055</v>
       </c>
       <c r="BA54" s="13">
-        <v>339055</v>
+        <v>446171</v>
       </c>
       <c r="BB54" s="13">
-        <v>446171</v>
+        <v>359620</v>
       </c>
     </row>
     <row r="55" spans="2:54" x14ac:dyDescent="0.3">
@@ -7225,8 +7225,8 @@
       <c r="AD56" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AE56" s="17" t="s">
-        <v>57</v>
+      <c r="AE56" s="17">
+        <v>0</v>
       </c>
       <c r="AF56" s="17">
         <v>0</v>
@@ -7441,8 +7441,8 @@
       <c r="AD58" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="AE58" s="17" t="s">
-        <v>57</v>
+      <c r="AE58" s="17">
+        <v>0</v>
       </c>
       <c r="AF58" s="17">
         <v>0</v>
@@ -7657,8 +7657,8 @@
       <c r="AD60" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AE60" s="11" t="s">
-        <v>57</v>
+      <c r="AE60" s="11">
+        <v>0</v>
       </c>
       <c r="AF60" s="11">
         <v>0</v>
@@ -7703,31 +7703,31 @@
         <v>0</v>
       </c>
       <c r="AT60" s="11">
-        <v>0</v>
+        <v>-222689</v>
       </c>
       <c r="AU60" s="11">
-        <v>-222689</v>
+        <v>-282220</v>
       </c>
       <c r="AV60" s="11">
-        <v>-282220</v>
+        <v>-298449</v>
       </c>
       <c r="AW60" s="11">
-        <v>-298449</v>
+        <v>-275998</v>
       </c>
       <c r="AX60" s="11">
-        <v>-275998</v>
+        <v>-326330</v>
       </c>
       <c r="AY60" s="11">
-        <v>-326330</v>
+        <v>-405203</v>
       </c>
       <c r="AZ60" s="11">
-        <v>-405203</v>
+        <v>-475225</v>
       </c>
       <c r="BA60" s="11">
-        <v>-475225</v>
+        <v>-417374</v>
       </c>
       <c r="BB60" s="11">
-        <v>-417374</v>
+        <v>-363051</v>
       </c>
     </row>
     <row r="61" spans="2:54" x14ac:dyDescent="0.3">
@@ -7737,154 +7737,154 @@
       <c r="C61" s="19"/>
       <c r="D61" s="19"/>
       <c r="E61" s="19">
-        <v>569703</v>
+        <v>600831</v>
       </c>
       <c r="F61" s="19">
-        <v>600831</v>
+        <v>537350</v>
       </c>
       <c r="G61" s="19">
-        <v>537350</v>
+        <v>577120</v>
       </c>
       <c r="H61" s="19">
-        <v>577120</v>
+        <v>664694</v>
       </c>
       <c r="I61" s="19">
-        <v>664694</v>
+        <v>715394</v>
       </c>
       <c r="J61" s="19">
-        <v>715394</v>
+        <v>475764</v>
       </c>
       <c r="K61" s="19">
-        <v>475764</v>
+        <v>858329</v>
       </c>
       <c r="L61" s="19">
-        <v>858329</v>
+        <v>672618</v>
       </c>
       <c r="M61" s="19">
-        <v>672618</v>
+        <v>779909</v>
       </c>
       <c r="N61" s="19">
-        <v>779909</v>
+        <v>740480</v>
       </c>
       <c r="O61" s="19">
-        <v>740480</v>
+        <v>875547</v>
       </c>
       <c r="P61" s="19">
-        <v>875547</v>
+        <v>1001359</v>
       </c>
       <c r="Q61" s="19">
-        <v>1001359</v>
+        <v>928842</v>
       </c>
       <c r="R61" s="19">
-        <v>928842</v>
+        <v>1101910</v>
       </c>
       <c r="S61" s="19">
-        <v>1101910</v>
+        <v>1061901</v>
       </c>
       <c r="T61" s="19">
-        <v>1061901</v>
+        <v>1120496</v>
       </c>
       <c r="U61" s="19">
-        <v>1120496</v>
+        <v>1175405</v>
       </c>
       <c r="V61" s="19">
-        <v>1175405</v>
+        <v>596894</v>
       </c>
       <c r="W61" s="19">
-        <v>596894</v>
+        <v>1054926</v>
       </c>
       <c r="X61" s="19">
-        <v>1054926</v>
+        <v>1018595</v>
       </c>
       <c r="Y61" s="19">
-        <v>1018595</v>
+        <v>1192044</v>
       </c>
       <c r="Z61" s="19">
-        <v>1192044</v>
+        <v>1307954</v>
       </c>
       <c r="AA61" s="19">
-        <v>1307954</v>
+        <v>1443904</v>
       </c>
       <c r="AB61" s="19">
-        <v>1443904</v>
+        <v>1632923</v>
       </c>
       <c r="AC61" s="19">
-        <v>1632923</v>
+        <v>1660605</v>
       </c>
       <c r="AD61" s="19">
-        <v>1660605</v>
+        <v>1517663</v>
       </c>
       <c r="AE61" s="19">
-        <v>1517663</v>
+        <v>1238213</v>
       </c>
       <c r="AF61" s="19">
-        <v>1238213</v>
+        <v>1503585</v>
       </c>
       <c r="AG61" s="19">
-        <v>1503585</v>
+        <v>1801298</v>
       </c>
       <c r="AH61" s="19">
-        <v>1801298</v>
+        <v>1100240</v>
       </c>
       <c r="AI61" s="19">
-        <v>1100240</v>
+        <v>1695682</v>
       </c>
       <c r="AJ61" s="19">
-        <v>1695682</v>
+        <v>1683999</v>
       </c>
       <c r="AK61" s="19">
-        <v>1683999</v>
+        <v>1909100</v>
       </c>
       <c r="AL61" s="19">
-        <v>1909100</v>
+        <v>2186584</v>
       </c>
       <c r="AM61" s="19">
-        <v>2186584</v>
+        <v>2807139</v>
       </c>
       <c r="AN61" s="19">
-        <v>2807139</v>
+        <v>2144282</v>
       </c>
       <c r="AO61" s="19">
-        <v>2144282</v>
+        <v>2643641</v>
       </c>
       <c r="AP61" s="19">
-        <v>2643641</v>
+        <v>2844859</v>
       </c>
       <c r="AQ61" s="19">
-        <v>2844859</v>
+        <v>2318869</v>
       </c>
       <c r="AR61" s="19">
-        <v>2318869</v>
+        <v>3100486</v>
       </c>
       <c r="AS61" s="19">
-        <v>3100486</v>
+        <v>2789248</v>
       </c>
       <c r="AT61" s="19">
-        <v>2789248</v>
+        <v>2123721</v>
       </c>
       <c r="AU61" s="19">
-        <v>2123721</v>
+        <v>3019752</v>
       </c>
       <c r="AV61" s="19">
-        <v>3019752</v>
+        <v>3013224</v>
       </c>
       <c r="AW61" s="19">
-        <v>3013224</v>
+        <v>3236139</v>
       </c>
       <c r="AX61" s="19">
-        <v>3236139</v>
+        <v>3953272</v>
       </c>
       <c r="AY61" s="19">
-        <v>3953272</v>
+        <v>4349855</v>
       </c>
       <c r="AZ61" s="19">
-        <v>4349855</v>
+        <v>4909511</v>
       </c>
       <c r="BA61" s="19">
-        <v>4909511</v>
+        <v>5680258</v>
       </c>
       <c r="BB61" s="19">
-        <v>5680258</v>
+        <v>5527063</v>
       </c>
     </row>
     <row r="62" spans="2:54" x14ac:dyDescent="0.3">
@@ -8443,41 +8443,41 @@
       <c r="AP68" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AQ68" s="11" t="s">
-        <v>57</v>
+      <c r="AQ68" s="11">
+        <v>611111</v>
       </c>
       <c r="AR68" s="11">
-        <v>611111</v>
+        <v>608696</v>
       </c>
       <c r="AS68" s="11">
-        <v>608696</v>
-      </c>
-      <c r="AT68" s="11">
         <v>602410</v>
       </c>
-      <c r="AU68" s="11" t="s">
-        <v>57</v>
+      <c r="AT68" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="AU68" s="11">
+        <v>632310</v>
       </c>
       <c r="AV68" s="11">
-        <v>632310</v>
+        <v>632158</v>
       </c>
       <c r="AW68" s="11">
-        <v>632158</v>
+        <v>632340</v>
       </c>
       <c r="AX68" s="11">
-        <v>632340</v>
+        <v>632468</v>
       </c>
       <c r="AY68" s="11">
-        <v>632468</v>
+        <v>1584068</v>
       </c>
       <c r="AZ68" s="11">
-        <v>1584068</v>
+        <v>704874</v>
       </c>
       <c r="BA68" s="11">
-        <v>704874</v>
+        <v>572880</v>
       </c>
       <c r="BB68" s="11">
-        <v>572880</v>
+        <v>1017829</v>
       </c>
     </row>
     <row r="69" spans="2:54" x14ac:dyDescent="0.3">
@@ -8512,8 +8512,8 @@
       <c r="L69" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="M69" s="13" t="s">
-        <v>57</v>
+      <c r="M69" s="13">
+        <v>0</v>
       </c>
       <c r="N69" s="13">
         <v>0</v>
@@ -8530,8 +8530,8 @@
       <c r="R69" s="13">
         <v>0</v>
       </c>
-      <c r="S69" s="13">
-        <v>0</v>
+      <c r="S69" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="T69" s="13" t="s">
         <v>57</v>
@@ -8539,35 +8539,35 @@
       <c r="U69" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="V69" s="13" t="s">
-        <v>57</v>
+      <c r="V69" s="13">
+        <v>604167</v>
       </c>
       <c r="W69" s="13">
-        <v>604167</v>
+        <v>0</v>
       </c>
       <c r="X69" s="13">
         <v>0</v>
       </c>
       <c r="Y69" s="13">
-        <v>0</v>
+        <v>607143</v>
       </c>
       <c r="Z69" s="13">
-        <v>607143</v>
+        <v>607873</v>
       </c>
       <c r="AA69" s="13">
-        <v>607873</v>
+        <v>603008</v>
       </c>
       <c r="AB69" s="13">
-        <v>603008</v>
+        <v>595368</v>
       </c>
       <c r="AC69" s="13">
-        <v>595368</v>
+        <v>539836</v>
       </c>
       <c r="AD69" s="13">
-        <v>539836</v>
-      </c>
-      <c r="AE69" s="13">
         <v>603537</v>
+      </c>
+      <c r="AE69" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AF69" s="13" t="s">
         <v>57</v>
@@ -8648,59 +8648,59 @@
       </c>
       <c r="D70" s="11"/>
       <c r="E70" s="11">
-        <v>760870</v>
+        <v>791746</v>
       </c>
       <c r="F70" s="11">
-        <v>791746</v>
+        <v>778310</v>
       </c>
       <c r="G70" s="11">
-        <v>778310</v>
+        <v>795697</v>
       </c>
       <c r="H70" s="11">
-        <v>795697</v>
+        <v>793974</v>
       </c>
       <c r="I70" s="11">
-        <v>793974</v>
+        <v>689067</v>
       </c>
       <c r="J70" s="11">
-        <v>689067</v>
+        <v>805434</v>
       </c>
       <c r="K70" s="11">
-        <v>805434</v>
+        <v>801962</v>
       </c>
       <c r="L70" s="11">
-        <v>801962</v>
+        <v>798831</v>
       </c>
       <c r="M70" s="11">
-        <v>798831</v>
+        <v>804589</v>
       </c>
       <c r="N70" s="11">
-        <v>804589</v>
+        <v>613756</v>
       </c>
       <c r="O70" s="11">
-        <v>613756</v>
+        <v>608484</v>
       </c>
       <c r="P70" s="11">
-        <v>608484</v>
+        <v>558792</v>
       </c>
       <c r="Q70" s="11">
-        <v>558792</v>
+        <v>561587</v>
       </c>
       <c r="R70" s="11">
-        <v>561587</v>
+        <v>584189</v>
       </c>
       <c r="S70" s="11">
-        <v>584189</v>
+        <v>571553</v>
       </c>
       <c r="T70" s="11">
-        <v>571553</v>
+        <v>594512</v>
       </c>
       <c r="U70" s="11">
-        <v>594512</v>
-      </c>
-      <c r="V70" s="11">
         <v>592403</v>
       </c>
+      <c r="V70" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="W70" s="11" t="s">
         <v>57</v>
       </c>
@@ -8725,44 +8725,44 @@
       <c r="AD70" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AE70" s="11" t="s">
-        <v>57</v>
+      <c r="AE70" s="11">
+        <v>602527</v>
       </c>
       <c r="AF70" s="11">
-        <v>602527</v>
+        <v>541851</v>
       </c>
       <c r="AG70" s="11">
-        <v>541851</v>
+        <v>568779</v>
       </c>
       <c r="AH70" s="11">
-        <v>568779</v>
+        <v>579625</v>
       </c>
       <c r="AI70" s="11">
-        <v>579625</v>
+        <v>615528</v>
       </c>
       <c r="AJ70" s="11">
-        <v>615528</v>
+        <v>605450</v>
       </c>
       <c r="AK70" s="11">
-        <v>605450</v>
+        <v>547128</v>
       </c>
       <c r="AL70" s="11">
-        <v>547128</v>
+        <v>603844</v>
       </c>
       <c r="AM70" s="11">
-        <v>603844</v>
+        <v>604903</v>
       </c>
       <c r="AN70" s="11">
-        <v>604903</v>
+        <v>568216</v>
       </c>
       <c r="AO70" s="11">
-        <v>568216</v>
+        <v>601399</v>
       </c>
       <c r="AP70" s="11">
-        <v>601399</v>
-      </c>
-      <c r="AQ70" s="11">
         <v>603896</v>
+      </c>
+      <c r="AQ70" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="AR70" s="11" t="s">
         <v>57</v>
@@ -8807,121 +8807,121 @@
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="13">
-        <v>35210</v>
+        <v>33478</v>
       </c>
       <c r="F71" s="13">
-        <v>33478</v>
+        <v>34282</v>
       </c>
       <c r="G71" s="13">
-        <v>34282</v>
+        <v>38027</v>
       </c>
       <c r="H71" s="13">
-        <v>38027</v>
+        <v>43101</v>
       </c>
       <c r="I71" s="13">
-        <v>43101</v>
+        <v>40560</v>
       </c>
       <c r="J71" s="13">
-        <v>40560</v>
+        <v>52075</v>
       </c>
       <c r="K71" s="13">
-        <v>52075</v>
+        <v>44745</v>
       </c>
       <c r="L71" s="13">
-        <v>44745</v>
+        <v>54484</v>
       </c>
       <c r="M71" s="13">
-        <v>54484</v>
+        <v>51211</v>
       </c>
       <c r="N71" s="13">
-        <v>51211</v>
+        <v>55957</v>
       </c>
       <c r="O71" s="13">
-        <v>55957</v>
+        <v>55071</v>
       </c>
       <c r="P71" s="13">
-        <v>55071</v>
+        <v>62229</v>
       </c>
       <c r="Q71" s="13">
-        <v>62229</v>
+        <v>59406</v>
       </c>
       <c r="R71" s="13">
-        <v>59406</v>
+        <v>68996</v>
       </c>
       <c r="S71" s="13">
-        <v>68996</v>
+        <v>58986</v>
       </c>
       <c r="T71" s="13">
-        <v>58986</v>
+        <v>61756</v>
       </c>
       <c r="U71" s="13">
-        <v>61756</v>
+        <v>65786</v>
       </c>
       <c r="V71" s="13">
-        <v>65786</v>
+        <v>64360</v>
       </c>
       <c r="W71" s="13">
-        <v>64360</v>
+        <v>62704</v>
       </c>
       <c r="X71" s="13">
-        <v>62704</v>
+        <v>63634</v>
       </c>
       <c r="Y71" s="13">
-        <v>63634</v>
+        <v>61196</v>
       </c>
       <c r="Z71" s="13">
-        <v>61196</v>
+        <v>63628</v>
       </c>
       <c r="AA71" s="13">
-        <v>63628</v>
+        <v>88795</v>
       </c>
       <c r="AB71" s="13">
-        <v>88795</v>
+        <v>87867</v>
       </c>
       <c r="AC71" s="13">
-        <v>87867</v>
+        <v>106932</v>
       </c>
       <c r="AD71" s="13">
-        <v>106932</v>
+        <v>88003</v>
       </c>
       <c r="AE71" s="13">
-        <v>88003</v>
+        <v>90906</v>
       </c>
       <c r="AF71" s="13">
-        <v>90906</v>
+        <v>81221</v>
       </c>
       <c r="AG71" s="13">
-        <v>81221</v>
+        <v>85602</v>
       </c>
       <c r="AH71" s="13">
-        <v>85602</v>
+        <v>96999</v>
       </c>
       <c r="AI71" s="13">
-        <v>96999</v>
+        <v>88526</v>
       </c>
       <c r="AJ71" s="13">
-        <v>88526</v>
+        <v>89029</v>
       </c>
       <c r="AK71" s="13">
-        <v>89029</v>
+        <v>87690</v>
       </c>
       <c r="AL71" s="13">
-        <v>87690</v>
+        <v>83798</v>
       </c>
       <c r="AM71" s="13">
-        <v>83798</v>
+        <v>92042</v>
       </c>
       <c r="AN71" s="13">
-        <v>92042</v>
+        <v>93642</v>
       </c>
       <c r="AO71" s="13">
-        <v>93642</v>
+        <v>94136</v>
       </c>
       <c r="AP71" s="13">
-        <v>94136</v>
-      </c>
-      <c r="AQ71" s="13">
         <v>96235</v>
+      </c>
+      <c r="AQ71" s="13" t="s">
+        <v>57</v>
       </c>
       <c r="AR71" s="13" t="s">
         <v>57</v>
@@ -8966,154 +8966,154 @@
       </c>
       <c r="D72" s="11"/>
       <c r="E72" s="11">
-        <v>343107</v>
+        <v>288793</v>
       </c>
       <c r="F72" s="11">
-        <v>288793</v>
+        <v>363768</v>
       </c>
       <c r="G72" s="11">
-        <v>363768</v>
+        <v>314950</v>
       </c>
       <c r="H72" s="11">
-        <v>314950</v>
+        <v>358206</v>
       </c>
       <c r="I72" s="11">
-        <v>358206</v>
+        <v>370938</v>
       </c>
       <c r="J72" s="11">
-        <v>370938</v>
+        <v>403898</v>
       </c>
       <c r="K72" s="11">
-        <v>403898</v>
+        <v>363807</v>
       </c>
       <c r="L72" s="11">
-        <v>363807</v>
+        <v>415351</v>
       </c>
       <c r="M72" s="11">
-        <v>415351</v>
+        <v>400448</v>
       </c>
       <c r="N72" s="11">
-        <v>400448</v>
+        <v>378249</v>
       </c>
       <c r="O72" s="11">
-        <v>378249</v>
+        <v>450119</v>
       </c>
       <c r="P72" s="11">
-        <v>450119</v>
+        <v>332020</v>
       </c>
       <c r="Q72" s="11">
-        <v>332020</v>
+        <v>269334</v>
       </c>
       <c r="R72" s="11">
-        <v>269334</v>
+        <v>363441</v>
       </c>
       <c r="S72" s="11">
-        <v>363441</v>
+        <v>348745</v>
       </c>
       <c r="T72" s="11">
-        <v>348745</v>
+        <v>364322</v>
       </c>
       <c r="U72" s="11">
-        <v>364322</v>
+        <v>408123</v>
       </c>
       <c r="V72" s="11">
-        <v>408123</v>
+        <v>422548</v>
       </c>
       <c r="W72" s="11">
-        <v>422548</v>
+        <v>394136</v>
       </c>
       <c r="X72" s="11">
-        <v>394136</v>
+        <v>429354</v>
       </c>
       <c r="Y72" s="11">
-        <v>429354</v>
+        <v>393139</v>
       </c>
       <c r="Z72" s="11">
-        <v>393139</v>
+        <v>424261</v>
       </c>
       <c r="AA72" s="11">
-        <v>424261</v>
+        <v>465730</v>
       </c>
       <c r="AB72" s="11">
-        <v>465730</v>
+        <v>424936</v>
       </c>
       <c r="AC72" s="11">
-        <v>424936</v>
+        <v>445970</v>
       </c>
       <c r="AD72" s="11">
-        <v>445970</v>
+        <v>505126</v>
       </c>
       <c r="AE72" s="11">
-        <v>505126</v>
+        <v>586468</v>
       </c>
       <c r="AF72" s="11">
-        <v>586468</v>
+        <v>645575</v>
       </c>
       <c r="AG72" s="11">
-        <v>645575</v>
+        <v>711391</v>
       </c>
       <c r="AH72" s="11">
-        <v>711391</v>
+        <v>736880</v>
       </c>
       <c r="AI72" s="11">
-        <v>736880</v>
+        <v>655700</v>
       </c>
       <c r="AJ72" s="11">
-        <v>655700</v>
+        <v>705447</v>
       </c>
       <c r="AK72" s="11">
-        <v>705447</v>
+        <v>664425</v>
       </c>
       <c r="AL72" s="11">
-        <v>664425</v>
+        <v>741118</v>
       </c>
       <c r="AM72" s="11">
-        <v>741118</v>
+        <v>550356</v>
       </c>
       <c r="AN72" s="11">
-        <v>550356</v>
+        <v>770494</v>
       </c>
       <c r="AO72" s="11">
-        <v>770494</v>
+        <v>810130</v>
       </c>
       <c r="AP72" s="11">
-        <v>810130</v>
+        <v>854335</v>
       </c>
       <c r="AQ72" s="11">
-        <v>854335</v>
+        <v>771224</v>
       </c>
       <c r="AR72" s="11">
-        <v>771224</v>
+        <v>677694</v>
       </c>
       <c r="AS72" s="11">
-        <v>677694</v>
+        <v>784398</v>
       </c>
       <c r="AT72" s="11">
-        <v>784398</v>
+        <v>1003401</v>
       </c>
       <c r="AU72" s="11">
-        <v>1003401</v>
+        <v>794890</v>
       </c>
       <c r="AV72" s="11">
-        <v>794890</v>
+        <v>1035767</v>
       </c>
       <c r="AW72" s="11">
-        <v>1035767</v>
+        <v>946353</v>
       </c>
       <c r="AX72" s="11">
-        <v>946353</v>
+        <v>1086246</v>
       </c>
       <c r="AY72" s="11">
-        <v>1086246</v>
+        <v>1287793</v>
       </c>
       <c r="AZ72" s="11">
-        <v>1287793</v>
+        <v>801982</v>
       </c>
       <c r="BA72" s="11">
-        <v>801982</v>
+        <v>1192348</v>
       </c>
       <c r="BB72" s="11">
-        <v>1192348</v>
+        <v>1229658</v>
       </c>
     </row>
     <row r="73" spans="2:54" x14ac:dyDescent="0.3">
@@ -9125,154 +9125,154 @@
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="13">
-        <v>261484</v>
+        <v>290611</v>
       </c>
       <c r="F73" s="13">
-        <v>290611</v>
+        <v>232504</v>
       </c>
       <c r="G73" s="13">
-        <v>232504</v>
+        <v>260970</v>
       </c>
       <c r="H73" s="13">
-        <v>260970</v>
+        <v>368832</v>
       </c>
       <c r="I73" s="13">
-        <v>368832</v>
+        <v>462956</v>
       </c>
       <c r="J73" s="13">
-        <v>462956</v>
+        <v>445536</v>
       </c>
       <c r="K73" s="13">
-        <v>445536</v>
+        <v>433188</v>
       </c>
       <c r="L73" s="13">
-        <v>433188</v>
+        <v>497728</v>
       </c>
       <c r="M73" s="13">
-        <v>497728</v>
+        <v>522092</v>
       </c>
       <c r="N73" s="13">
-        <v>522092</v>
+        <v>458548</v>
       </c>
       <c r="O73" s="13">
-        <v>458548</v>
+        <v>304119</v>
       </c>
       <c r="P73" s="13">
-        <v>304119</v>
+        <v>502078</v>
       </c>
       <c r="Q73" s="13">
-        <v>502078</v>
+        <v>338918</v>
       </c>
       <c r="R73" s="13">
-        <v>338918</v>
+        <v>446045</v>
       </c>
       <c r="S73" s="13">
-        <v>446045</v>
+        <v>413835</v>
       </c>
       <c r="T73" s="13">
-        <v>413835</v>
+        <v>527815</v>
       </c>
       <c r="U73" s="13">
-        <v>527815</v>
+        <v>543233</v>
       </c>
       <c r="V73" s="13">
-        <v>543233</v>
+        <v>557176</v>
       </c>
       <c r="W73" s="13">
-        <v>557176</v>
+        <v>515585</v>
       </c>
       <c r="X73" s="13">
-        <v>515585</v>
+        <v>577606</v>
       </c>
       <c r="Y73" s="13">
-        <v>577606</v>
+        <v>577925</v>
       </c>
       <c r="Z73" s="13">
-        <v>577925</v>
+        <v>581963</v>
       </c>
       <c r="AA73" s="13">
-        <v>581963</v>
+        <v>380532</v>
       </c>
       <c r="AB73" s="13">
-        <v>380532</v>
+        <v>638640</v>
       </c>
       <c r="AC73" s="13">
-        <v>638640</v>
+        <v>688077</v>
       </c>
       <c r="AD73" s="13">
-        <v>688077</v>
+        <v>651967</v>
       </c>
       <c r="AE73" s="13">
-        <v>651967</v>
+        <v>849169</v>
       </c>
       <c r="AF73" s="13">
-        <v>849169</v>
+        <v>814198</v>
       </c>
       <c r="AG73" s="13">
-        <v>814198</v>
+        <v>880393</v>
       </c>
       <c r="AH73" s="13">
-        <v>880393</v>
+        <v>952669</v>
       </c>
       <c r="AI73" s="13">
-        <v>952669</v>
+        <v>906939</v>
       </c>
       <c r="AJ73" s="13">
-        <v>906939</v>
+        <v>974935</v>
       </c>
       <c r="AK73" s="13">
-        <v>974935</v>
+        <v>830298</v>
       </c>
       <c r="AL73" s="13">
-        <v>830298</v>
+        <v>807358</v>
       </c>
       <c r="AM73" s="13">
-        <v>807358</v>
+        <v>829821</v>
       </c>
       <c r="AN73" s="13">
-        <v>829821</v>
+        <v>879101</v>
       </c>
       <c r="AO73" s="13">
-        <v>879101</v>
+        <v>788274</v>
       </c>
       <c r="AP73" s="13">
-        <v>788274</v>
+        <v>914407</v>
       </c>
       <c r="AQ73" s="13">
-        <v>914407</v>
+        <v>815405</v>
       </c>
       <c r="AR73" s="13">
-        <v>815405</v>
+        <v>720796</v>
       </c>
       <c r="AS73" s="13">
-        <v>720796</v>
+        <v>839116</v>
       </c>
       <c r="AT73" s="13">
-        <v>839116</v>
+        <v>974841</v>
       </c>
       <c r="AU73" s="13">
-        <v>974841</v>
+        <v>1030911</v>
       </c>
       <c r="AV73" s="13">
-        <v>1030911</v>
+        <v>1065335</v>
       </c>
       <c r="AW73" s="13">
-        <v>1065335</v>
+        <v>1100646</v>
       </c>
       <c r="AX73" s="13">
-        <v>1100646</v>
+        <v>1493168</v>
       </c>
       <c r="AY73" s="13">
-        <v>1493168</v>
+        <v>1431849</v>
       </c>
       <c r="AZ73" s="13">
-        <v>1431849</v>
+        <v>1302553</v>
       </c>
       <c r="BA73" s="13">
-        <v>1302553</v>
+        <v>1521305</v>
       </c>
       <c r="BB73" s="13">
-        <v>1521305</v>
+        <v>1677388</v>
       </c>
     </row>
     <row r="74" spans="2:54" x14ac:dyDescent="0.3">
@@ -9289,11 +9289,11 @@
       <c r="F74" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G74" s="11" t="s">
-        <v>57</v>
+      <c r="G74" s="11">
+        <v>10732</v>
       </c>
       <c r="H74" s="11">
-        <v>10732</v>
+        <v>0</v>
       </c>
       <c r="I74" s="11">
         <v>0</v>
@@ -9325,8 +9325,8 @@
       <c r="R74" s="11">
         <v>0</v>
       </c>
-      <c r="S74" s="11">
-        <v>0</v>
+      <c r="S74" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="T74" s="11" t="s">
         <v>57</v>
@@ -9556,41 +9556,41 @@
       <c r="AP75" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="AQ75" s="13" t="s">
-        <v>57</v>
+      <c r="AQ75" s="13">
+        <v>93138</v>
       </c>
       <c r="AR75" s="13">
-        <v>93138</v>
+        <v>98344</v>
       </c>
       <c r="AS75" s="13">
-        <v>98344</v>
+        <v>104604</v>
       </c>
       <c r="AT75" s="13">
-        <v>104604</v>
+        <v>123902</v>
       </c>
       <c r="AU75" s="13">
-        <v>123902</v>
+        <v>123093</v>
       </c>
       <c r="AV75" s="13">
-        <v>123093</v>
+        <v>125251</v>
       </c>
       <c r="AW75" s="13">
-        <v>125251</v>
+        <v>127980</v>
       </c>
       <c r="AX75" s="13">
-        <v>127980</v>
+        <v>135077</v>
       </c>
       <c r="AY75" s="13">
-        <v>135077</v>
+        <v>132702</v>
       </c>
       <c r="AZ75" s="13">
-        <v>132702</v>
+        <v>131910</v>
       </c>
       <c r="BA75" s="13">
-        <v>131910</v>
+        <v>178484</v>
       </c>
       <c r="BB75" s="13">
-        <v>178484</v>
+        <v>183972</v>
       </c>
     </row>
   </sheetData>

</xml_diff>